<commit_message>
updated excel file with CWs
</commit_message>
<xml_diff>
--- a/ctrl words dlx.xlsx
+++ b/ctrl words dlx.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tinar\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kelme\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F374F4C4-134A-482F-874E-DE3A2BEBCA57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF54695-5923-4B13-B59C-49BDBB4AF9C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{97E78207-76B4-4719-AF3A-2C20865B08CC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{97E78207-76B4-4719-AF3A-2C20865B08CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="71">
   <si>
     <t>BranchD</t>
   </si>
@@ -238,6 +238,15 @@
   </si>
   <si>
     <t>branch</t>
+  </si>
+  <si>
+    <t>Comp_control</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>10</t>
   </si>
 </sst>
 </file>
@@ -653,7 +662,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="199">
+  <cellXfs count="209">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
@@ -775,12 +784,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -889,9 +892,41 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normale 2" xfId="1" xr:uid="{0BE64102-23FE-4CD4-BAA4-AEBC2824A2EF}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -922,7 +957,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1221,10 +1256,10 @@
   <dimension ref="A1:T68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E61" sqref="E61"/>
+      <selection pane="bottomRight" activeCell="X55" sqref="X55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1232,7 +1267,7 @@
     <col min="3" max="3" width="11.28515625" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="145"/>
+    <col min="8" max="8" width="9.140625" style="143"/>
     <col min="16" max="16" width="12.28515625" customWidth="1"/>
     <col min="17" max="17" width="12.140625" customWidth="1"/>
     <col min="20" max="20" width="14.28515625" customWidth="1"/>
@@ -1257,25 +1292,28 @@
       <c r="G1" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="132" t="s">
+      <c r="H1" s="130" t="s">
         <v>26</v>
       </c>
       <c r="I1" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="121" t="s">
+      <c r="J1" s="197" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="121"/>
-      <c r="L1" s="121"/>
-      <c r="M1" s="121"/>
-      <c r="N1" s="121"/>
-      <c r="O1" s="121"/>
+      <c r="K1" s="197"/>
+      <c r="L1" s="197"/>
+      <c r="M1" s="197"/>
+      <c r="N1" s="197"/>
+      <c r="O1" s="197"/>
       <c r="P1" s="22" t="s">
         <v>29</v>
       </c>
       <c r="Q1" s="23" t="s">
         <v>2</v>
+      </c>
+      <c r="R1" s="199" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1300,7 +1338,7 @@
       <c r="G2" s="26">
         <v>1</v>
       </c>
-      <c r="H2" s="133">
+      <c r="H2" s="131">
         <v>1</v>
       </c>
       <c r="I2" s="26">
@@ -1329,6 +1367,9 @@
       </c>
       <c r="Q2" s="31">
         <v>0</v>
+      </c>
+      <c r="R2" s="200" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -1353,7 +1394,7 @@
       <c r="G3" s="26">
         <v>1</v>
       </c>
-      <c r="H3" s="133">
+      <c r="H3" s="131">
         <v>1</v>
       </c>
       <c r="I3" s="26">
@@ -1383,10 +1424,13 @@
       <c r="Q3" s="31">
         <v>0</v>
       </c>
-      <c r="S3" s="122" t="s">
+      <c r="R3" s="200" t="s">
+        <v>69</v>
+      </c>
+      <c r="S3" s="198" t="s">
         <v>53</v>
       </c>
-      <c r="T3" s="122"/>
+      <c r="T3" s="198"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
@@ -1410,7 +1454,7 @@
       <c r="G4" s="26">
         <v>1</v>
       </c>
-      <c r="H4" s="133">
+      <c r="H4" s="131">
         <v>1</v>
       </c>
       <c r="I4" s="26">
@@ -1439,6 +1483,9 @@
       </c>
       <c r="Q4" s="31">
         <v>0</v>
+      </c>
+      <c r="R4" s="200" t="s">
+        <v>69</v>
       </c>
       <c r="S4" s="41"/>
       <c r="T4" t="s">
@@ -1467,7 +1514,7 @@
       <c r="G5" s="26">
         <v>1</v>
       </c>
-      <c r="H5" s="133">
+      <c r="H5" s="131">
         <v>1</v>
       </c>
       <c r="I5" s="26">
@@ -1496,6 +1543,9 @@
       </c>
       <c r="Q5" s="31">
         <v>0</v>
+      </c>
+      <c r="R5" s="200" t="s">
+        <v>69</v>
       </c>
       <c r="S5" s="59"/>
       <c r="T5" t="s">
@@ -1524,7 +1574,7 @@
       <c r="G6" s="26">
         <v>1</v>
       </c>
-      <c r="H6" s="133">
+      <c r="H6" s="131">
         <v>1</v>
       </c>
       <c r="I6" s="26">
@@ -1553,6 +1603,9 @@
       </c>
       <c r="Q6" s="31">
         <v>0</v>
+      </c>
+      <c r="R6" s="200" t="s">
+        <v>69</v>
       </c>
       <c r="S6" s="76"/>
       <c r="T6" t="s">
@@ -1581,7 +1634,7 @@
       <c r="G7" s="34">
         <v>1</v>
       </c>
-      <c r="H7" s="134">
+      <c r="H7" s="132">
         <v>1</v>
       </c>
       <c r="I7" s="34">
@@ -1610,6 +1663,9 @@
       </c>
       <c r="Q7" s="39">
         <v>0</v>
+      </c>
+      <c r="R7" s="200" t="s">
+        <v>69</v>
       </c>
       <c r="S7" s="93"/>
       <c r="T7" t="s">
@@ -1638,7 +1694,7 @@
       <c r="G8" s="26">
         <v>0</v>
       </c>
-      <c r="H8" s="133">
+      <c r="H8" s="131">
         <v>0</v>
       </c>
       <c r="I8" s="26">
@@ -1667,6 +1723,9 @@
       </c>
       <c r="Q8" s="31">
         <v>0</v>
+      </c>
+      <c r="R8" s="200" t="s">
+        <v>69</v>
       </c>
       <c r="S8" s="103"/>
       <c r="T8" t="s">
@@ -1695,7 +1754,7 @@
       <c r="G9" s="26">
         <v>0</v>
       </c>
-      <c r="H9" s="133">
+      <c r="H9" s="131">
         <v>0</v>
       </c>
       <c r="I9" s="26">
@@ -1724,6 +1783,9 @@
       </c>
       <c r="Q9" s="31">
         <v>0</v>
+      </c>
+      <c r="R9" s="200" t="s">
+        <v>69</v>
       </c>
       <c r="S9" s="120"/>
       <c r="T9" t="s">
@@ -1752,7 +1814,7 @@
       <c r="G10" s="26">
         <v>0</v>
       </c>
-      <c r="H10" s="133">
+      <c r="H10" s="131">
         <v>0</v>
       </c>
       <c r="I10" s="26">
@@ -1782,7 +1844,10 @@
       <c r="Q10" s="31">
         <v>0</v>
       </c>
-      <c r="S10" s="148"/>
+      <c r="R10" s="200" t="s">
+        <v>69</v>
+      </c>
+      <c r="S10" s="146"/>
       <c r="T10" t="s">
         <v>41</v>
       </c>
@@ -1809,7 +1874,7 @@
       <c r="G11" s="26">
         <v>0</v>
       </c>
-      <c r="H11" s="133">
+      <c r="H11" s="131">
         <v>0</v>
       </c>
       <c r="I11" s="26">
@@ -1839,7 +1904,10 @@
       <c r="Q11" s="31">
         <v>0</v>
       </c>
-      <c r="S11" s="160"/>
+      <c r="R11" s="200" t="s">
+        <v>69</v>
+      </c>
+      <c r="S11" s="158"/>
       <c r="T11" t="s">
         <v>66</v>
       </c>
@@ -1866,7 +1934,7 @@
       <c r="G12" s="26">
         <v>0</v>
       </c>
-      <c r="H12" s="133">
+      <c r="H12" s="131">
         <v>0</v>
       </c>
       <c r="I12" s="26">
@@ -1896,7 +1964,10 @@
       <c r="Q12" s="31">
         <v>0</v>
       </c>
-      <c r="S12" s="182"/>
+      <c r="R12" s="200" t="s">
+        <v>69</v>
+      </c>
+      <c r="S12" s="180"/>
       <c r="T12" t="s">
         <v>67</v>
       </c>
@@ -1923,7 +1994,7 @@
       <c r="G13" s="34">
         <v>0</v>
       </c>
-      <c r="H13" s="134">
+      <c r="H13" s="132">
         <v>0</v>
       </c>
       <c r="I13" s="34">
@@ -1952,6 +2023,9 @@
       </c>
       <c r="Q13" s="39">
         <v>0</v>
+      </c>
+      <c r="R13" s="200" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -1962,7 +2036,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="6"/>
-      <c r="H14" s="135"/>
+      <c r="H14" s="133"/>
       <c r="I14" s="6"/>
       <c r="J14" s="11"/>
       <c r="K14" s="12"/>
@@ -1995,7 +2069,7 @@
       <c r="G15" s="44">
         <v>1</v>
       </c>
-      <c r="H15" s="136">
+      <c r="H15" s="134">
         <v>1</v>
       </c>
       <c r="I15" s="44">
@@ -2024,6 +2098,9 @@
       </c>
       <c r="Q15" s="49">
         <v>0</v>
+      </c>
+      <c r="R15" s="201" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -2048,7 +2125,7 @@
       <c r="G16" s="44">
         <v>1</v>
       </c>
-      <c r="H16" s="136">
+      <c r="H16" s="134">
         <v>1</v>
       </c>
       <c r="I16" s="44">
@@ -2078,8 +2155,11 @@
       <c r="Q16" s="49">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R16" s="201" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="50" t="s">
         <v>44</v>
       </c>
@@ -2101,7 +2181,7 @@
       <c r="G17" s="44">
         <v>0</v>
       </c>
-      <c r="H17" s="136">
+      <c r="H17" s="134">
         <v>0</v>
       </c>
       <c r="I17" s="44">
@@ -2131,8 +2211,11 @@
       <c r="Q17" s="49">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R17" s="201" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="51" t="s">
         <v>45</v>
       </c>
@@ -2154,7 +2237,7 @@
       <c r="G18" s="53">
         <v>0</v>
       </c>
-      <c r="H18" s="137">
+      <c r="H18" s="135">
         <v>0</v>
       </c>
       <c r="I18" s="53">
@@ -2184,8 +2267,11 @@
       <c r="Q18" s="58">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R18" s="201" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="10"/>
       <c r="C19" s="5"/>
@@ -2193,7 +2279,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="135"/>
+      <c r="H19" s="133"/>
       <c r="I19" s="6"/>
       <c r="J19" s="11">
         <v>0</v>
@@ -2216,7 +2302,7 @@
       <c r="P19" s="6"/>
       <c r="Q19" s="7"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="60" t="s">
         <v>10</v>
       </c>
@@ -2238,7 +2324,7 @@
       <c r="G20" s="62">
         <v>1</v>
       </c>
-      <c r="H20" s="138">
+      <c r="H20" s="136">
         <v>1</v>
       </c>
       <c r="I20" s="62">
@@ -2268,8 +2354,11 @@
       <c r="Q20" s="67">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R20" s="202" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="60" t="s">
         <v>11</v>
       </c>
@@ -2291,7 +2380,7 @@
       <c r="G21" s="62">
         <v>1</v>
       </c>
-      <c r="H21" s="138">
+      <c r="H21" s="136">
         <v>1</v>
       </c>
       <c r="I21" s="62">
@@ -2321,8 +2410,11 @@
       <c r="Q21" s="67">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R21" s="202" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="60" t="s">
         <v>12</v>
       </c>
@@ -2344,7 +2436,7 @@
       <c r="G22" s="62">
         <v>1</v>
       </c>
-      <c r="H22" s="138">
+      <c r="H22" s="136">
         <v>1</v>
       </c>
       <c r="I22" s="62">
@@ -2374,8 +2466,11 @@
       <c r="Q22" s="67">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R22" s="202" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="68" t="s">
         <v>13</v>
       </c>
@@ -2397,7 +2492,7 @@
       <c r="G23" s="70">
         <v>1</v>
       </c>
-      <c r="H23" s="139">
+      <c r="H23" s="137">
         <v>1</v>
       </c>
       <c r="I23" s="70">
@@ -2427,8 +2522,11 @@
       <c r="Q23" s="75">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R23" s="202" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="60" t="s">
         <v>30</v>
       </c>
@@ -2450,7 +2548,7 @@
       <c r="G24" s="62">
         <v>0</v>
       </c>
-      <c r="H24" s="138">
+      <c r="H24" s="136">
         <v>0</v>
       </c>
       <c r="I24" s="62">
@@ -2480,8 +2578,11 @@
       <c r="Q24" s="67">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R24" s="202" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="60" t="s">
         <v>31</v>
       </c>
@@ -2503,7 +2604,7 @@
       <c r="G25" s="62">
         <v>0</v>
       </c>
-      <c r="H25" s="138">
+      <c r="H25" s="136">
         <v>0</v>
       </c>
       <c r="I25" s="62">
@@ -2533,8 +2634,11 @@
       <c r="Q25" s="67">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R25" s="202" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="60" t="s">
         <v>32</v>
       </c>
@@ -2556,7 +2660,7 @@
       <c r="G26" s="62">
         <v>0</v>
       </c>
-      <c r="H26" s="138">
+      <c r="H26" s="136">
         <v>0</v>
       </c>
       <c r="I26" s="62">
@@ -2586,8 +2690,11 @@
       <c r="Q26" s="67">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R26" s="202" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="68" t="s">
         <v>33</v>
       </c>
@@ -2609,7 +2716,7 @@
       <c r="G27" s="70">
         <v>0</v>
       </c>
-      <c r="H27" s="139">
+      <c r="H27" s="137">
         <v>0</v>
       </c>
       <c r="I27" s="70">
@@ -2639,8 +2746,11 @@
       <c r="Q27" s="75">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R27" s="202" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="10"/>
       <c r="C28" s="5"/>
@@ -2648,7 +2758,7 @@
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="6"/>
-      <c r="H28" s="135"/>
+      <c r="H28" s="133"/>
       <c r="I28" s="6"/>
       <c r="J28" s="11"/>
       <c r="K28" s="12"/>
@@ -2659,7 +2769,7 @@
       <c r="P28" s="6"/>
       <c r="Q28" s="7"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="77" t="s">
         <v>35</v>
       </c>
@@ -2681,7 +2791,7 @@
       <c r="G29" s="79">
         <v>1</v>
       </c>
-      <c r="H29" s="140">
+      <c r="H29" s="138">
         <v>1</v>
       </c>
       <c r="I29" s="79">
@@ -2711,8 +2821,11 @@
       <c r="Q29" s="84">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R29" s="203" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="77" t="s">
         <v>34</v>
       </c>
@@ -2734,7 +2847,7 @@
       <c r="G30" s="79">
         <v>1</v>
       </c>
-      <c r="H30" s="140">
+      <c r="H30" s="138">
         <v>1</v>
       </c>
       <c r="I30" s="79">
@@ -2764,8 +2877,11 @@
       <c r="Q30" s="84">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R30" s="203" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="77" t="s">
         <v>36</v>
       </c>
@@ -2787,7 +2903,7 @@
       <c r="G31" s="79">
         <v>1</v>
       </c>
-      <c r="H31" s="140">
+      <c r="H31" s="138">
         <v>1</v>
       </c>
       <c r="I31" s="79">
@@ -2817,8 +2933,11 @@
       <c r="Q31" s="84">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R31" s="203" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="77" t="s">
         <v>14</v>
       </c>
@@ -2840,7 +2959,7 @@
       <c r="G32" s="79">
         <v>1</v>
       </c>
-      <c r="H32" s="140">
+      <c r="H32" s="138">
         <v>1</v>
       </c>
       <c r="I32" s="79">
@@ -2870,8 +2989,11 @@
       <c r="Q32" s="84">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R32" s="203" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="77" t="s">
         <v>37</v>
       </c>
@@ -2893,7 +3015,7 @@
       <c r="G33" s="79">
         <v>1</v>
       </c>
-      <c r="H33" s="140">
+      <c r="H33" s="138">
         <v>1</v>
       </c>
       <c r="I33" s="79">
@@ -2923,8 +3045,11 @@
       <c r="Q33" s="84">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R33" s="203" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="77" t="s">
         <v>15</v>
       </c>
@@ -2946,7 +3071,7 @@
       <c r="G34" s="79">
         <v>1</v>
       </c>
-      <c r="H34" s="140">
+      <c r="H34" s="138">
         <v>1</v>
       </c>
       <c r="I34" s="79">
@@ -2976,8 +3101,11 @@
       <c r="Q34" s="84">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R34" s="203" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="85" t="s">
         <v>38</v>
       </c>
@@ -2999,7 +3127,7 @@
       <c r="G35" s="87">
         <v>1</v>
       </c>
-      <c r="H35" s="147">
+      <c r="H35" s="145">
         <v>1</v>
       </c>
       <c r="I35" s="87">
@@ -3029,8 +3157,11 @@
       <c r="Q35" s="92">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R35" s="203" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="77" t="s">
         <v>46</v>
       </c>
@@ -3052,7 +3183,7 @@
       <c r="G36" s="79">
         <v>0</v>
       </c>
-      <c r="H36" s="140">
+      <c r="H36" s="138">
         <v>0</v>
       </c>
       <c r="I36" s="79">
@@ -3082,8 +3213,11 @@
       <c r="Q36" s="84">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R36" s="203" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="77" t="s">
         <v>47</v>
       </c>
@@ -3105,7 +3239,7 @@
       <c r="G37" s="79">
         <v>0</v>
       </c>
-      <c r="H37" s="140">
+      <c r="H37" s="138">
         <v>0</v>
       </c>
       <c r="I37" s="79">
@@ -3135,8 +3269,11 @@
       <c r="Q37" s="84">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R37" s="203" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="77" t="s">
         <v>48</v>
       </c>
@@ -3158,7 +3295,7 @@
       <c r="G38" s="79">
         <v>0</v>
       </c>
-      <c r="H38" s="140">
+      <c r="H38" s="138">
         <v>0</v>
       </c>
       <c r="I38" s="79">
@@ -3188,8 +3325,11 @@
       <c r="Q38" s="84">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R38" s="203" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="77" t="s">
         <v>49</v>
       </c>
@@ -3211,7 +3351,7 @@
       <c r="G39" s="79">
         <v>0</v>
       </c>
-      <c r="H39" s="140">
+      <c r="H39" s="138">
         <v>0</v>
       </c>
       <c r="I39" s="79">
@@ -3241,8 +3381,11 @@
       <c r="Q39" s="84">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R39" s="203" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="77" t="s">
         <v>50</v>
       </c>
@@ -3264,7 +3407,7 @@
       <c r="G40" s="79">
         <v>0</v>
       </c>
-      <c r="H40" s="140">
+      <c r="H40" s="138">
         <v>0</v>
       </c>
       <c r="I40" s="79">
@@ -3294,8 +3437,11 @@
       <c r="Q40" s="84">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R40" s="203" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="77" t="s">
         <v>51</v>
       </c>
@@ -3317,7 +3463,7 @@
       <c r="G41" s="79">
         <v>0</v>
       </c>
-      <c r="H41" s="140">
+      <c r="H41" s="138">
         <v>0</v>
       </c>
       <c r="I41" s="79">
@@ -3347,8 +3493,11 @@
       <c r="Q41" s="84">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R41" s="203" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="85" t="s">
         <v>52</v>
       </c>
@@ -3370,7 +3519,7 @@
       <c r="G42" s="87">
         <v>0</v>
       </c>
-      <c r="H42" s="140">
+      <c r="H42" s="138">
         <v>0</v>
       </c>
       <c r="I42" s="87">
@@ -3400,8 +3549,11 @@
       <c r="Q42" s="92">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R42" s="203" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="10"/>
       <c r="C43" s="5"/>
@@ -3409,7 +3561,7 @@
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="135"/>
+      <c r="H43" s="133"/>
       <c r="I43" s="6"/>
       <c r="J43" s="11"/>
       <c r="K43" s="12"/>
@@ -3420,60 +3572,63 @@
       <c r="P43" s="8"/>
       <c r="Q43" s="9"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A44" s="123" t="s">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A44" s="121" t="s">
         <v>16</v>
       </c>
-      <c r="B44" s="124">
-        <v>0</v>
-      </c>
-      <c r="C44" s="125">
-        <v>0</v>
-      </c>
-      <c r="D44" s="125">
-        <v>1</v>
-      </c>
-      <c r="E44" s="125">
-        <v>0</v>
-      </c>
-      <c r="F44" s="125">
-        <v>1</v>
-      </c>
-      <c r="G44" s="125">
-        <v>1</v>
-      </c>
-      <c r="H44" s="141">
-        <v>1</v>
-      </c>
-      <c r="I44" s="125">
-        <v>0</v>
-      </c>
-      <c r="J44" s="126">
-        <v>1</v>
-      </c>
-      <c r="K44" s="127">
-        <v>1</v>
-      </c>
-      <c r="L44" s="128">
-        <v>1</v>
-      </c>
-      <c r="M44" s="127">
-        <v>1</v>
-      </c>
-      <c r="N44" s="127">
-        <v>1</v>
-      </c>
-      <c r="O44" s="129">
-        <v>1</v>
-      </c>
-      <c r="P44" s="130">
-        <v>0</v>
-      </c>
-      <c r="Q44" s="131">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B44" s="122">
+        <v>0</v>
+      </c>
+      <c r="C44" s="123">
+        <v>0</v>
+      </c>
+      <c r="D44" s="123">
+        <v>1</v>
+      </c>
+      <c r="E44" s="123">
+        <v>0</v>
+      </c>
+      <c r="F44" s="123">
+        <v>1</v>
+      </c>
+      <c r="G44" s="123">
+        <v>1</v>
+      </c>
+      <c r="H44" s="139">
+        <v>1</v>
+      </c>
+      <c r="I44" s="123">
+        <v>0</v>
+      </c>
+      <c r="J44" s="124">
+        <v>1</v>
+      </c>
+      <c r="K44" s="125">
+        <v>1</v>
+      </c>
+      <c r="L44" s="126">
+        <v>1</v>
+      </c>
+      <c r="M44" s="125">
+        <v>1</v>
+      </c>
+      <c r="N44" s="125">
+        <v>1</v>
+      </c>
+      <c r="O44" s="127">
+        <v>1</v>
+      </c>
+      <c r="P44" s="128">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="129">
+        <v>0</v>
+      </c>
+      <c r="R44" s="208" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="94" t="s">
         <v>60</v>
       </c>
@@ -3495,7 +3650,7 @@
       <c r="G45" s="96">
         <v>0</v>
       </c>
-      <c r="H45" s="142">
+      <c r="H45" s="140">
         <v>0</v>
       </c>
       <c r="I45" s="96">
@@ -3525,8 +3680,11 @@
       <c r="Q45" s="102">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R45" s="208" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="10"/>
       <c r="C46" s="5"/>
@@ -3534,7 +3692,7 @@
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="135"/>
+      <c r="H46" s="133"/>
       <c r="I46" s="6"/>
       <c r="J46" s="14"/>
       <c r="K46" s="15"/>
@@ -3545,7 +3703,7 @@
       <c r="P46" s="6"/>
       <c r="Q46" s="7"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="104" t="s">
         <v>39</v>
       </c>
@@ -3567,7 +3725,7 @@
       <c r="G47" s="106">
         <v>0</v>
       </c>
-      <c r="H47" s="143">
+      <c r="H47" s="141">
         <v>0</v>
       </c>
       <c r="I47" s="106">
@@ -3597,8 +3755,11 @@
       <c r="Q47" s="111">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R47" s="205" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="112" t="s">
         <v>40</v>
       </c>
@@ -3620,7 +3781,7 @@
       <c r="G48" s="114">
         <v>0</v>
       </c>
-      <c r="H48" s="144">
+      <c r="H48" s="142">
         <v>0</v>
       </c>
       <c r="I48" s="114">
@@ -3650,8 +3811,11 @@
       <c r="Q48" s="119">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R48" s="205" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="10"/>
       <c r="C49" s="5"/>
@@ -3659,7 +3823,7 @@
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
       <c r="G49" s="6"/>
-      <c r="H49" s="135"/>
+      <c r="H49" s="133"/>
       <c r="I49" s="6"/>
       <c r="J49" s="17"/>
       <c r="K49" s="18"/>
@@ -3670,191 +3834,200 @@
       <c r="P49" s="6"/>
       <c r="Q49" s="7"/>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A50" s="149" t="s">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A50" s="147" t="s">
         <v>41</v>
       </c>
-      <c r="B50" s="150">
-        <v>0</v>
-      </c>
-      <c r="C50" s="151">
-        <v>0</v>
-      </c>
-      <c r="D50" s="151">
-        <v>0</v>
-      </c>
-      <c r="E50" s="151">
-        <v>0</v>
-      </c>
-      <c r="F50" s="151">
-        <v>0</v>
-      </c>
-      <c r="G50" s="151">
-        <v>0</v>
-      </c>
-      <c r="H50" s="152">
-        <v>0</v>
-      </c>
-      <c r="I50" s="151">
-        <v>0</v>
-      </c>
-      <c r="J50" s="153">
-        <v>0</v>
-      </c>
-      <c r="K50" s="154">
-        <v>0</v>
-      </c>
-      <c r="L50" s="154">
-        <v>0</v>
-      </c>
-      <c r="M50" s="154">
-        <v>0</v>
-      </c>
-      <c r="N50" s="154">
-        <v>0</v>
-      </c>
-      <c r="O50" s="155">
-        <v>0</v>
-      </c>
-      <c r="P50" s="151">
-        <v>0</v>
-      </c>
-      <c r="Q50" s="156">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A51" s="157"/>
-      <c r="B51" s="158"/>
-      <c r="C51" s="172"/>
+      <c r="B50" s="148">
+        <v>0</v>
+      </c>
+      <c r="C50" s="149">
+        <v>0</v>
+      </c>
+      <c r="D50" s="149">
+        <v>0</v>
+      </c>
+      <c r="E50" s="149">
+        <v>0</v>
+      </c>
+      <c r="F50" s="149">
+        <v>0</v>
+      </c>
+      <c r="G50" s="149">
+        <v>0</v>
+      </c>
+      <c r="H50" s="150">
+        <v>0</v>
+      </c>
+      <c r="I50" s="149">
+        <v>0</v>
+      </c>
+      <c r="J50" s="151">
+        <v>0</v>
+      </c>
+      <c r="K50" s="152">
+        <v>0</v>
+      </c>
+      <c r="L50" s="152">
+        <v>0</v>
+      </c>
+      <c r="M50" s="152">
+        <v>0</v>
+      </c>
+      <c r="N50" s="152">
+        <v>0</v>
+      </c>
+      <c r="O50" s="153">
+        <v>0</v>
+      </c>
+      <c r="P50" s="149">
+        <v>0</v>
+      </c>
+      <c r="Q50" s="154">
+        <v>0</v>
+      </c>
+      <c r="R50" s="206" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A51" s="155"/>
+      <c r="B51" s="156"/>
+      <c r="C51" s="170"/>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
-      <c r="H51" s="135"/>
+      <c r="H51" s="133"/>
       <c r="I51" s="6"/>
-      <c r="J51" s="173"/>
-      <c r="K51" s="174"/>
-      <c r="L51" s="174"/>
-      <c r="M51" s="174"/>
-      <c r="N51" s="174"/>
-      <c r="O51" s="175"/>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A52" s="161" t="s">
+      <c r="J51" s="171"/>
+      <c r="K51" s="172"/>
+      <c r="L51" s="172"/>
+      <c r="M51" s="172"/>
+      <c r="N51" s="172"/>
+      <c r="O51" s="173"/>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A52" s="159" t="s">
         <v>61</v>
       </c>
-      <c r="B52" s="162">
-        <v>1</v>
-      </c>
-      <c r="C52" s="165">
-        <v>1</v>
-      </c>
-      <c r="D52" s="165">
-        <v>0</v>
-      </c>
-      <c r="E52" s="165">
-        <v>0</v>
-      </c>
-      <c r="F52" s="165">
-        <v>0</v>
-      </c>
-      <c r="G52" s="165">
-        <v>0</v>
-      </c>
-      <c r="H52" s="166">
-        <v>0</v>
-      </c>
-      <c r="I52" s="165">
-        <v>0</v>
-      </c>
-      <c r="J52" s="176">
-        <v>0</v>
-      </c>
-      <c r="K52" s="177">
-        <v>0</v>
-      </c>
-      <c r="L52" s="177">
-        <v>0</v>
-      </c>
-      <c r="M52" s="177">
-        <v>0</v>
-      </c>
-      <c r="N52" s="177">
-        <v>0</v>
-      </c>
-      <c r="O52" s="180">
-        <v>0</v>
-      </c>
-      <c r="P52" s="165">
-        <v>0</v>
-      </c>
-      <c r="Q52" s="167">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A53" s="163" t="s">
+      <c r="B52" s="160">
+        <v>1</v>
+      </c>
+      <c r="C52" s="163">
+        <v>1</v>
+      </c>
+      <c r="D52" s="163">
+        <v>0</v>
+      </c>
+      <c r="E52" s="163">
+        <v>0</v>
+      </c>
+      <c r="F52" s="163">
+        <v>0</v>
+      </c>
+      <c r="G52" s="163">
+        <v>0</v>
+      </c>
+      <c r="H52" s="164">
+        <v>0</v>
+      </c>
+      <c r="I52" s="163">
+        <v>0</v>
+      </c>
+      <c r="J52" s="174">
+        <v>0</v>
+      </c>
+      <c r="K52" s="175">
+        <v>0</v>
+      </c>
+      <c r="L52" s="175">
+        <v>0</v>
+      </c>
+      <c r="M52" s="175">
+        <v>0</v>
+      </c>
+      <c r="N52" s="175">
+        <v>0</v>
+      </c>
+      <c r="O52" s="178">
+        <v>0</v>
+      </c>
+      <c r="P52" s="163">
+        <v>0</v>
+      </c>
+      <c r="Q52" s="165">
+        <v>0</v>
+      </c>
+      <c r="R52" s="207" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A53" s="161" t="s">
         <v>62</v>
       </c>
-      <c r="B53" s="164">
-        <v>1</v>
-      </c>
-      <c r="C53" s="168">
-        <v>1</v>
-      </c>
-      <c r="D53" s="168">
-        <v>1</v>
-      </c>
-      <c r="E53" s="168">
-        <v>1</v>
-      </c>
-      <c r="F53" s="168">
-        <v>0</v>
-      </c>
-      <c r="G53" s="168">
-        <v>0</v>
-      </c>
-      <c r="H53" s="169">
-        <v>0</v>
-      </c>
-      <c r="I53" s="168">
-        <v>0</v>
-      </c>
-      <c r="J53" s="178">
-        <v>0</v>
-      </c>
-      <c r="K53" s="179">
-        <v>0</v>
-      </c>
-      <c r="L53" s="179">
-        <v>0</v>
-      </c>
-      <c r="M53" s="179">
-        <v>0</v>
-      </c>
-      <c r="N53" s="179">
-        <v>0</v>
-      </c>
-      <c r="O53" s="181">
-        <v>0</v>
-      </c>
-      <c r="P53" s="168">
-        <v>0</v>
-      </c>
-      <c r="Q53" s="170">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B53" s="162">
+        <v>1</v>
+      </c>
+      <c r="C53" s="166">
+        <v>1</v>
+      </c>
+      <c r="D53" s="166">
+        <v>1</v>
+      </c>
+      <c r="E53" s="166">
+        <v>1</v>
+      </c>
+      <c r="F53" s="166">
+        <v>0</v>
+      </c>
+      <c r="G53" s="166">
+        <v>0</v>
+      </c>
+      <c r="H53" s="167">
+        <v>0</v>
+      </c>
+      <c r="I53" s="166">
+        <v>0</v>
+      </c>
+      <c r="J53" s="176">
+        <v>0</v>
+      </c>
+      <c r="K53" s="177">
+        <v>0</v>
+      </c>
+      <c r="L53" s="177">
+        <v>0</v>
+      </c>
+      <c r="M53" s="177">
+        <v>0</v>
+      </c>
+      <c r="N53" s="177">
+        <v>0</v>
+      </c>
+      <c r="O53" s="179">
+        <v>0</v>
+      </c>
+      <c r="P53" s="166">
+        <v>0</v>
+      </c>
+      <c r="Q53" s="168">
+        <v>0</v>
+      </c>
+      <c r="R53" s="207" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
-      <c r="B54" s="159"/>
+      <c r="B54" s="157"/>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
-      <c r="H54" s="171"/>
+      <c r="H54" s="169"/>
       <c r="I54" s="6"/>
       <c r="J54" s="17"/>
       <c r="K54" s="18"/>
@@ -3865,141 +4038,147 @@
       <c r="P54" s="6"/>
       <c r="Q54" s="7"/>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A55" s="183" t="s">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A55" s="181" t="s">
         <v>64</v>
       </c>
-      <c r="B55" s="184">
-        <v>1</v>
-      </c>
-      <c r="C55" s="185">
-        <v>1</v>
-      </c>
-      <c r="D55" s="185">
-        <v>0</v>
-      </c>
-      <c r="E55" s="185">
-        <v>0</v>
-      </c>
-      <c r="F55" s="185">
-        <v>1</v>
-      </c>
-      <c r="G55" s="185">
-        <v>1</v>
-      </c>
-      <c r="H55" s="186">
-        <v>0</v>
-      </c>
-      <c r="I55" s="186">
-        <v>0</v>
-      </c>
-      <c r="J55" s="187">
-        <v>0</v>
-      </c>
-      <c r="K55" s="188">
-        <v>0</v>
-      </c>
-      <c r="L55" s="188">
-        <v>0</v>
-      </c>
-      <c r="M55" s="188">
-        <v>0</v>
-      </c>
-      <c r="N55" s="188">
-        <v>0</v>
-      </c>
-      <c r="O55" s="189">
-        <v>0</v>
-      </c>
-      <c r="P55" s="185">
-        <v>0</v>
-      </c>
-      <c r="Q55" s="190">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A56" s="191" t="s">
+      <c r="B55" s="182">
+        <v>1</v>
+      </c>
+      <c r="C55" s="183">
+        <v>1</v>
+      </c>
+      <c r="D55" s="183">
+        <v>0</v>
+      </c>
+      <c r="E55" s="183">
+        <v>0</v>
+      </c>
+      <c r="F55" s="183">
+        <v>1</v>
+      </c>
+      <c r="G55" s="183">
+        <v>1</v>
+      </c>
+      <c r="H55" s="184">
+        <v>0</v>
+      </c>
+      <c r="I55" s="184">
+        <v>0</v>
+      </c>
+      <c r="J55" s="185">
+        <v>0</v>
+      </c>
+      <c r="K55" s="186">
+        <v>0</v>
+      </c>
+      <c r="L55" s="186">
+        <v>0</v>
+      </c>
+      <c r="M55" s="186">
+        <v>0</v>
+      </c>
+      <c r="N55" s="186">
+        <v>0</v>
+      </c>
+      <c r="O55" s="187">
+        <v>0</v>
+      </c>
+      <c r="P55" s="183">
+        <v>0</v>
+      </c>
+      <c r="Q55" s="188">
+        <v>0</v>
+      </c>
+      <c r="R55" s="204">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A56" s="189" t="s">
         <v>65</v>
       </c>
-      <c r="B56" s="192">
-        <v>1</v>
-      </c>
-      <c r="C56" s="193">
-        <v>1</v>
-      </c>
-      <c r="D56" s="193">
-        <v>0</v>
-      </c>
-      <c r="E56" s="193">
-        <v>0</v>
-      </c>
-      <c r="F56" s="193">
-        <v>1</v>
-      </c>
-      <c r="G56" s="193">
-        <v>1</v>
-      </c>
-      <c r="H56" s="194">
-        <v>0</v>
-      </c>
-      <c r="I56" s="194">
-        <v>0</v>
-      </c>
-      <c r="J56" s="195">
-        <v>0</v>
-      </c>
-      <c r="K56" s="196">
-        <v>0</v>
-      </c>
-      <c r="L56" s="196">
-        <v>0</v>
-      </c>
-      <c r="M56" s="196">
-        <v>0</v>
-      </c>
-      <c r="N56" s="196">
-        <v>0</v>
-      </c>
-      <c r="O56" s="197">
-        <v>0</v>
-      </c>
-      <c r="P56" s="193">
-        <v>0</v>
-      </c>
-      <c r="Q56" s="198">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A57" s="146"/>
+      <c r="B56" s="190">
+        <v>1</v>
+      </c>
+      <c r="C56" s="191">
+        <v>1</v>
+      </c>
+      <c r="D56" s="191">
+        <v>0</v>
+      </c>
+      <c r="E56" s="191">
+        <v>0</v>
+      </c>
+      <c r="F56" s="191">
+        <v>1</v>
+      </c>
+      <c r="G56" s="191">
+        <v>1</v>
+      </c>
+      <c r="H56" s="192">
+        <v>0</v>
+      </c>
+      <c r="I56" s="192">
+        <v>0</v>
+      </c>
+      <c r="J56" s="193">
+        <v>0</v>
+      </c>
+      <c r="K56" s="194">
+        <v>0</v>
+      </c>
+      <c r="L56" s="194">
+        <v>0</v>
+      </c>
+      <c r="M56" s="194">
+        <v>0</v>
+      </c>
+      <c r="N56" s="194">
+        <v>0</v>
+      </c>
+      <c r="O56" s="195">
+        <v>0</v>
+      </c>
+      <c r="P56" s="191">
+        <v>0</v>
+      </c>
+      <c r="Q56" s="196">
+        <v>0</v>
+      </c>
+      <c r="R56" s="204">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A57" s="144"/>
       <c r="B57" s="4"/>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
     </row>

</xml_diff>

<commit_message>
fixed select_ext for branches
</commit_message>
<xml_diff>
--- a/ctrl words dlx.xlsx
+++ b/ctrl words dlx.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kelme\Desktop\DLX AUGUST\DLXproj\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kelme\Desktop\DLX_git\DLXproj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7644AF1C-2DD5-4654-9362-3C60514EB85D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B26B704-AD56-4AED-9CBF-1E25B47E6283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{97E78207-76B4-4719-AF3A-2C20865B08CC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{97E78207-76B4-4719-AF3A-2C20865B08CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -1259,21 +1259,21 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S53" sqref="S53"/>
+      <selection pane="bottomRight" activeCell="H65" sqref="H65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="143"/>
-    <col min="16" max="16" width="12.28515625" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" customWidth="1"/>
-    <col min="20" max="20" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" style="143"/>
+    <col min="16" max="16" width="12.33203125" customWidth="1"/>
+    <col min="17" max="17" width="12.109375" customWidth="1"/>
+    <col min="20" max="20" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="20" t="s">
         <v>0</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="24" t="s">
         <v>4</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
         <v>5</v>
       </c>
@@ -1432,7 +1432,7 @@
       </c>
       <c r="T3" s="208"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
         <v>6</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
         <v>7</v>
       </c>
@@ -1552,7 +1552,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="24" t="s">
         <v>8</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="32" t="s">
         <v>9</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="24" t="s">
         <v>17</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="24" t="s">
         <v>18</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="24" t="s">
         <v>19</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="24" t="s">
         <v>20</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
         <v>21</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="32" t="s">
         <v>22</v>
       </c>
@@ -2028,7 +2028,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="10"/>
       <c r="C14" s="5"/>
@@ -2047,7 +2047,7 @@
       <c r="P14" s="8"/>
       <c r="Q14" s="9"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="42" t="s">
         <v>42</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="50" t="s">
         <v>43</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="50" t="s">
         <v>44</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="51" t="s">
         <v>45</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="10"/>
       <c r="C19" s="5"/>
@@ -2302,7 +2302,7 @@
       <c r="P19" s="6"/>
       <c r="Q19" s="7"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="60" t="s">
         <v>10</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="60" t="s">
         <v>11</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="60" t="s">
         <v>12</v>
       </c>
@@ -2470,7 +2470,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="68" t="s">
         <v>13</v>
       </c>
@@ -2526,7 +2526,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="60" t="s">
         <v>30</v>
       </c>
@@ -2582,7 +2582,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="60" t="s">
         <v>31</v>
       </c>
@@ -2638,7 +2638,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="60" t="s">
         <v>32</v>
       </c>
@@ -2694,7 +2694,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="68" t="s">
         <v>33</v>
       </c>
@@ -2750,7 +2750,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="10"/>
       <c r="C28" s="5"/>
@@ -2769,7 +2769,7 @@
       <c r="P28" s="6"/>
       <c r="Q28" s="7"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="77" t="s">
         <v>35</v>
       </c>
@@ -2825,7 +2825,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="77" t="s">
         <v>34</v>
       </c>
@@ -2881,7 +2881,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="77" t="s">
         <v>36</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="77" t="s">
         <v>14</v>
       </c>
@@ -2993,7 +2993,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="77" t="s">
         <v>37</v>
       </c>
@@ -3049,7 +3049,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="77" t="s">
         <v>15</v>
       </c>
@@ -3105,7 +3105,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="85" t="s">
         <v>38</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="77" t="s">
         <v>46</v>
       </c>
@@ -3217,7 +3217,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="77" t="s">
         <v>47</v>
       </c>
@@ -3273,7 +3273,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="77" t="s">
         <v>48</v>
       </c>
@@ -3329,7 +3329,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="77" t="s">
         <v>49</v>
       </c>
@@ -3385,7 +3385,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" s="77" t="s">
         <v>50</v>
       </c>
@@ -3441,7 +3441,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" s="77" t="s">
         <v>51</v>
       </c>
@@ -3497,7 +3497,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="85" t="s">
         <v>52</v>
       </c>
@@ -3553,7 +3553,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="10"/>
       <c r="C43" s="5"/>
@@ -3572,7 +3572,7 @@
       <c r="P43" s="8"/>
       <c r="Q43" s="9"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="121" t="s">
         <v>16</v>
       </c>
@@ -3628,7 +3628,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="94" t="s">
         <v>60</v>
       </c>
@@ -3684,7 +3684,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
       <c r="B46" s="10"/>
       <c r="C46" s="5"/>
@@ -3703,7 +3703,7 @@
       <c r="P46" s="6"/>
       <c r="Q46" s="7"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="104" t="s">
         <v>39</v>
       </c>
@@ -3759,7 +3759,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="112" t="s">
         <v>40</v>
       </c>
@@ -3815,7 +3815,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" s="3"/>
       <c r="B49" s="10"/>
       <c r="C49" s="5"/>
@@ -3834,7 +3834,7 @@
       <c r="P49" s="6"/>
       <c r="Q49" s="7"/>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50" s="147" t="s">
         <v>41</v>
       </c>
@@ -3890,7 +3890,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" s="155"/>
       <c r="B51" s="156"/>
       <c r="C51" s="170"/>
@@ -3907,7 +3907,7 @@
       <c r="N51" s="172"/>
       <c r="O51" s="173"/>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52" s="159" t="s">
         <v>61</v>
       </c>
@@ -3963,7 +3963,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53" s="161" t="s">
         <v>62</v>
       </c>
@@ -4019,7 +4019,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" s="3"/>
       <c r="B54" s="157"/>
       <c r="C54" s="6"/>
@@ -4038,7 +4038,7 @@
       <c r="P54" s="6"/>
       <c r="Q54" s="7"/>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55" s="181" t="s">
         <v>64</v>
       </c>
@@ -4046,7 +4046,7 @@
         <v>1</v>
       </c>
       <c r="C55" s="183">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D55" s="183">
         <v>0</v>
@@ -4094,7 +4094,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56" s="189" t="s">
         <v>65</v>
       </c>
@@ -4102,7 +4102,7 @@
         <v>1</v>
       </c>
       <c r="C56" s="191">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D56" s="191">
         <v>0</v>
@@ -4150,51 +4150,51 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57" s="144"/>
       <c r="B57" s="4"/>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel and design updated with alu enable
</commit_message>
<xml_diff>
--- a/ctrl words dlx.xlsx
+++ b/ctrl words dlx.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kelme\Desktop\DLX_git\DLXproj\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kelme\Desktop\DLX_git2\DLXproj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B26B704-AD56-4AED-9CBF-1E25B47E6283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FF2F6A-87DF-41E0-98FA-EC3FA221A683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{97E78207-76B4-4719-AF3A-2C20865B08CC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="72">
   <si>
     <t>BranchD</t>
   </si>
@@ -247,6 +247,9 @@
   </si>
   <si>
     <t>01</t>
+  </si>
+  <si>
+    <t>en_ALU</t>
   </si>
 </sst>
 </file>
@@ -662,7 +665,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="209">
+  <cellXfs count="223">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
@@ -924,6 +927,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1253,13 +1270,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FA04DC4-AE17-4075-AF88-F2CFFC720BD3}">
-  <dimension ref="A1:T68"/>
+  <dimension ref="A1:U68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H65" sqref="H65"/>
+      <selection pane="bottomRight" activeCell="W50" sqref="W50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1268,12 +1285,12 @@
     <col min="4" max="4" width="11.6640625" customWidth="1"/>
     <col min="5" max="5" width="9.5546875" customWidth="1"/>
     <col min="8" max="8" width="9.109375" style="143"/>
-    <col min="16" max="16" width="12.33203125" customWidth="1"/>
-    <col min="17" max="17" width="12.109375" customWidth="1"/>
-    <col min="20" max="20" width="14.33203125" customWidth="1"/>
+    <col min="17" max="17" width="12.33203125" customWidth="1"/>
+    <col min="18" max="18" width="12.109375" customWidth="1"/>
+    <col min="21" max="21" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="20" t="s">
         <v>0</v>
       </c>
@@ -1298,25 +1315,28 @@
       <c r="I1" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="207" t="s">
+      <c r="J1" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="K1" s="207" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="207"/>
       <c r="L1" s="207"/>
       <c r="M1" s="207"/>
       <c r="N1" s="207"/>
       <c r="O1" s="207"/>
-      <c r="P1" s="22" t="s">
+      <c r="P1" s="207"/>
+      <c r="Q1" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="23" t="s">
+      <c r="R1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="197" t="s">
+      <c r="S1" s="197" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="24" t="s">
         <v>4</v>
       </c>
@@ -1344,35 +1364,38 @@
       <c r="I2" s="26">
         <v>0</v>
       </c>
-      <c r="J2" s="27">
-        <v>0</v>
-      </c>
-      <c r="K2" s="28">
+      <c r="J2" s="209">
+        <v>1</v>
+      </c>
+      <c r="K2" s="27">
         <v>0</v>
       </c>
       <c r="L2" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2" s="28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N2" s="28">
         <v>0</v>
       </c>
-      <c r="O2" s="29">
-        <v>0</v>
-      </c>
-      <c r="P2" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="31">
-        <v>0</v>
-      </c>
-      <c r="R2" s="198" t="s">
+      <c r="O2" s="28">
+        <v>0</v>
+      </c>
+      <c r="P2" s="29">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="30">
+        <v>0</v>
+      </c>
+      <c r="R2" s="31">
+        <v>0</v>
+      </c>
+      <c r="S2" s="198" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
         <v>5</v>
       </c>
@@ -1400,14 +1423,14 @@
       <c r="I3" s="26">
         <v>0</v>
       </c>
-      <c r="J3" s="27">
-        <v>0</v>
-      </c>
-      <c r="K3" s="28">
+      <c r="J3" s="209">
+        <v>1</v>
+      </c>
+      <c r="K3" s="27">
         <v>0</v>
       </c>
       <c r="L3" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3" s="28">
         <v>1</v>
@@ -1415,24 +1438,27 @@
       <c r="N3" s="28">
         <v>1</v>
       </c>
-      <c r="O3" s="29">
-        <v>0</v>
-      </c>
-      <c r="P3" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="31">
-        <v>0</v>
-      </c>
-      <c r="R3" s="198" t="s">
+      <c r="O3" s="28">
+        <v>1</v>
+      </c>
+      <c r="P3" s="29">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="30">
+        <v>0</v>
+      </c>
+      <c r="R3" s="31">
+        <v>0</v>
+      </c>
+      <c r="S3" s="198" t="s">
         <v>69</v>
       </c>
-      <c r="S3" s="208" t="s">
+      <c r="T3" s="208" t="s">
         <v>53</v>
       </c>
-      <c r="T3" s="208"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U3" s="208"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
         <v>6</v>
       </c>
@@ -1460,39 +1486,42 @@
       <c r="I4" s="26">
         <v>0</v>
       </c>
-      <c r="J4" s="27">
-        <v>0</v>
-      </c>
-      <c r="K4" s="28">
+      <c r="J4" s="209">
+        <v>1</v>
+      </c>
+      <c r="K4" s="27">
         <v>0</v>
       </c>
       <c r="L4" s="28">
         <v>0</v>
       </c>
       <c r="M4" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N4" s="28">
         <v>1</v>
       </c>
-      <c r="O4" s="29">
-        <v>0</v>
-      </c>
-      <c r="P4" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="31">
-        <v>0</v>
-      </c>
-      <c r="R4" s="198" t="s">
+      <c r="O4" s="28">
+        <v>1</v>
+      </c>
+      <c r="P4" s="29">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="30">
+        <v>0</v>
+      </c>
+      <c r="R4" s="31">
+        <v>0</v>
+      </c>
+      <c r="S4" s="198" t="s">
         <v>69</v>
       </c>
-      <c r="S4" s="41"/>
-      <c r="T4" t="s">
+      <c r="T4" s="41"/>
+      <c r="U4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
         <v>7</v>
       </c>
@@ -1520,39 +1549,42 @@
       <c r="I5" s="26">
         <v>0</v>
       </c>
-      <c r="J5" s="27">
-        <v>0</v>
-      </c>
-      <c r="K5" s="28">
+      <c r="J5" s="209">
+        <v>1</v>
+      </c>
+      <c r="K5" s="27">
         <v>0</v>
       </c>
       <c r="L5" s="28">
         <v>0</v>
       </c>
       <c r="M5" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N5" s="28">
         <v>1</v>
       </c>
-      <c r="O5" s="29">
-        <v>1</v>
-      </c>
-      <c r="P5" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="31">
-        <v>0</v>
-      </c>
-      <c r="R5" s="198" t="s">
+      <c r="O5" s="28">
+        <v>1</v>
+      </c>
+      <c r="P5" s="29">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="30">
+        <v>0</v>
+      </c>
+      <c r="R5" s="31">
+        <v>0</v>
+      </c>
+      <c r="S5" s="198" t="s">
         <v>69</v>
       </c>
-      <c r="S5" s="59"/>
-      <c r="T5" t="s">
+      <c r="T5" s="59"/>
+      <c r="U5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="24" t="s">
         <v>8</v>
       </c>
@@ -1580,10 +1612,10 @@
       <c r="I6" s="26">
         <v>0</v>
       </c>
-      <c r="J6" s="27">
-        <v>0</v>
-      </c>
-      <c r="K6" s="28">
+      <c r="J6" s="209">
+        <v>1</v>
+      </c>
+      <c r="K6" s="27">
         <v>0</v>
       </c>
       <c r="L6" s="28">
@@ -1595,24 +1627,27 @@
       <c r="N6" s="28">
         <v>0</v>
       </c>
-      <c r="O6" s="29">
-        <v>1</v>
-      </c>
-      <c r="P6" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="31">
-        <v>0</v>
-      </c>
-      <c r="R6" s="198" t="s">
+      <c r="O6" s="28">
+        <v>0</v>
+      </c>
+      <c r="P6" s="29">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="30">
+        <v>0</v>
+      </c>
+      <c r="R6" s="31">
+        <v>0</v>
+      </c>
+      <c r="S6" s="198" t="s">
         <v>69</v>
       </c>
-      <c r="S6" s="76"/>
-      <c r="T6" t="s">
+      <c r="T6" s="76"/>
+      <c r="U6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="32" t="s">
         <v>9</v>
       </c>
@@ -1640,39 +1675,42 @@
       <c r="I7" s="34">
         <v>0</v>
       </c>
-      <c r="J7" s="35">
-        <v>0</v>
-      </c>
-      <c r="K7" s="36">
+      <c r="J7" s="210">
+        <v>1</v>
+      </c>
+      <c r="K7" s="35">
         <v>0</v>
       </c>
       <c r="L7" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7" s="36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7" s="36">
         <v>0</v>
       </c>
-      <c r="O7" s="37">
-        <v>1</v>
-      </c>
-      <c r="P7" s="38">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="39">
-        <v>0</v>
-      </c>
-      <c r="R7" s="198" t="s">
+      <c r="O7" s="36">
+        <v>0</v>
+      </c>
+      <c r="P7" s="37">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="38">
+        <v>0</v>
+      </c>
+      <c r="R7" s="39">
+        <v>0</v>
+      </c>
+      <c r="S7" s="198" t="s">
         <v>69</v>
       </c>
-      <c r="S7" s="93"/>
-      <c r="T7" t="s">
+      <c r="T7" s="93"/>
+      <c r="U7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="24" t="s">
         <v>17</v>
       </c>
@@ -1700,39 +1738,42 @@
       <c r="I8" s="26">
         <v>1</v>
       </c>
-      <c r="J8" s="27">
-        <v>0</v>
-      </c>
-      <c r="K8" s="28">
+      <c r="J8" s="209">
+        <v>1</v>
+      </c>
+      <c r="K8" s="27">
         <v>0</v>
       </c>
       <c r="L8" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8" s="28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8" s="28">
         <v>0</v>
       </c>
-      <c r="O8" s="29">
-        <v>0</v>
-      </c>
-      <c r="P8" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="31">
-        <v>0</v>
-      </c>
-      <c r="R8" s="198" t="s">
+      <c r="O8" s="28">
+        <v>0</v>
+      </c>
+      <c r="P8" s="29">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="30">
+        <v>0</v>
+      </c>
+      <c r="R8" s="31">
+        <v>0</v>
+      </c>
+      <c r="S8" s="198" t="s">
         <v>69</v>
       </c>
-      <c r="S8" s="103"/>
-      <c r="T8" t="s">
+      <c r="T8" s="103"/>
+      <c r="U8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="24" t="s">
         <v>18</v>
       </c>
@@ -1760,14 +1801,14 @@
       <c r="I9" s="26">
         <v>1</v>
       </c>
-      <c r="J9" s="27">
-        <v>0</v>
-      </c>
-      <c r="K9" s="28">
+      <c r="J9" s="209">
+        <v>1</v>
+      </c>
+      <c r="K9" s="27">
         <v>0</v>
       </c>
       <c r="L9" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M9" s="28">
         <v>1</v>
@@ -1775,24 +1816,27 @@
       <c r="N9" s="28">
         <v>1</v>
       </c>
-      <c r="O9" s="29">
-        <v>0</v>
-      </c>
-      <c r="P9" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="31">
-        <v>0</v>
-      </c>
-      <c r="R9" s="198" t="s">
+      <c r="O9" s="28">
+        <v>1</v>
+      </c>
+      <c r="P9" s="29">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="30">
+        <v>0</v>
+      </c>
+      <c r="R9" s="31">
+        <v>0</v>
+      </c>
+      <c r="S9" s="198" t="s">
         <v>69</v>
       </c>
-      <c r="S9" s="120"/>
-      <c r="T9" t="s">
+      <c r="T9" s="120"/>
+      <c r="U9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="24" t="s">
         <v>19</v>
       </c>
@@ -1820,39 +1864,42 @@
       <c r="I10" s="26">
         <v>1</v>
       </c>
-      <c r="J10" s="27">
-        <v>0</v>
-      </c>
-      <c r="K10" s="28">
+      <c r="J10" s="209">
+        <v>1</v>
+      </c>
+      <c r="K10" s="27">
         <v>0</v>
       </c>
       <c r="L10" s="28">
         <v>0</v>
       </c>
       <c r="M10" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N10" s="28">
         <v>1</v>
       </c>
-      <c r="O10" s="29">
-        <v>0</v>
-      </c>
-      <c r="P10" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="31">
-        <v>0</v>
-      </c>
-      <c r="R10" s="198" t="s">
+      <c r="O10" s="28">
+        <v>1</v>
+      </c>
+      <c r="P10" s="29">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="30">
+        <v>0</v>
+      </c>
+      <c r="R10" s="31">
+        <v>0</v>
+      </c>
+      <c r="S10" s="198" t="s">
         <v>69</v>
       </c>
-      <c r="S10" s="146"/>
-      <c r="T10" t="s">
+      <c r="T10" s="146"/>
+      <c r="U10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="24" t="s">
         <v>20</v>
       </c>
@@ -1880,39 +1927,42 @@
       <c r="I11" s="26">
         <v>1</v>
       </c>
-      <c r="J11" s="27">
-        <v>0</v>
-      </c>
-      <c r="K11" s="28">
+      <c r="J11" s="209">
+        <v>1</v>
+      </c>
+      <c r="K11" s="27">
         <v>0</v>
       </c>
       <c r="L11" s="28">
         <v>0</v>
       </c>
       <c r="M11" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N11" s="28">
         <v>1</v>
       </c>
-      <c r="O11" s="29">
-        <v>1</v>
-      </c>
-      <c r="P11" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="31">
-        <v>0</v>
-      </c>
-      <c r="R11" s="198" t="s">
+      <c r="O11" s="28">
+        <v>1</v>
+      </c>
+      <c r="P11" s="29">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="30">
+        <v>0</v>
+      </c>
+      <c r="R11" s="31">
+        <v>0</v>
+      </c>
+      <c r="S11" s="198" t="s">
         <v>69</v>
       </c>
-      <c r="S11" s="158"/>
-      <c r="T11" t="s">
+      <c r="T11" s="158"/>
+      <c r="U11" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
         <v>21</v>
       </c>
@@ -1940,10 +1990,10 @@
       <c r="I12" s="26">
         <v>1</v>
       </c>
-      <c r="J12" s="27">
-        <v>0</v>
-      </c>
-      <c r="K12" s="28">
+      <c r="J12" s="209">
+        <v>1</v>
+      </c>
+      <c r="K12" s="27">
         <v>0</v>
       </c>
       <c r="L12" s="28">
@@ -1955,24 +2005,27 @@
       <c r="N12" s="28">
         <v>0</v>
       </c>
-      <c r="O12" s="29">
-        <v>1</v>
-      </c>
-      <c r="P12" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="31">
-        <v>0</v>
-      </c>
-      <c r="R12" s="198" t="s">
+      <c r="O12" s="28">
+        <v>0</v>
+      </c>
+      <c r="P12" s="29">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="30">
+        <v>0</v>
+      </c>
+      <c r="R12" s="31">
+        <v>0</v>
+      </c>
+      <c r="S12" s="198" t="s">
         <v>69</v>
       </c>
-      <c r="S12" s="180"/>
-      <c r="T12" t="s">
+      <c r="T12" s="180"/>
+      <c r="U12" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="32" t="s">
         <v>22</v>
       </c>
@@ -2000,35 +2053,38 @@
       <c r="I13" s="34">
         <v>1</v>
       </c>
-      <c r="J13" s="35">
-        <v>0</v>
-      </c>
-      <c r="K13" s="36">
+      <c r="J13" s="210">
+        <v>1</v>
+      </c>
+      <c r="K13" s="35">
         <v>0</v>
       </c>
       <c r="L13" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13" s="36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13" s="36">
         <v>0</v>
       </c>
-      <c r="O13" s="37">
-        <v>1</v>
-      </c>
-      <c r="P13" s="38">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="39">
-        <v>0</v>
-      </c>
-      <c r="R13" s="198" t="s">
+      <c r="O13" s="36">
+        <v>0</v>
+      </c>
+      <c r="P13" s="37">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="38">
+        <v>0</v>
+      </c>
+      <c r="R13" s="39">
+        <v>0</v>
+      </c>
+      <c r="S13" s="198" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="10"/>
       <c r="C14" s="5"/>
@@ -2038,16 +2094,17 @@
       <c r="G14" s="6"/>
       <c r="H14" s="133"/>
       <c r="I14" s="6"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="12"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="11"/>
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
       <c r="N14" s="12"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="9"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="O14" s="12"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="9"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="42" t="s">
         <v>42</v>
       </c>
@@ -2075,35 +2132,38 @@
       <c r="I15" s="44">
         <v>0</v>
       </c>
-      <c r="J15" s="45">
-        <v>0</v>
-      </c>
-      <c r="K15" s="46">
-        <v>1</v>
-      </c>
-      <c r="L15" s="46" t="s">
+      <c r="J15" s="211">
+        <v>1</v>
+      </c>
+      <c r="K15" s="45">
+        <v>0</v>
+      </c>
+      <c r="L15" s="46">
+        <v>1</v>
+      </c>
+      <c r="M15" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="M15" s="46">
-        <v>0</v>
-      </c>
       <c r="N15" s="46">
         <v>0</v>
       </c>
-      <c r="O15" s="47">
-        <v>0</v>
-      </c>
-      <c r="P15" s="48">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="49">
-        <v>0</v>
-      </c>
-      <c r="R15" s="199" t="s">
+      <c r="O15" s="46">
+        <v>0</v>
+      </c>
+      <c r="P15" s="47">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="48">
+        <v>0</v>
+      </c>
+      <c r="R15" s="49">
+        <v>0</v>
+      </c>
+      <c r="S15" s="199" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="50" t="s">
         <v>43</v>
       </c>
@@ -2131,35 +2191,38 @@
       <c r="I16" s="44">
         <v>0</v>
       </c>
-      <c r="J16" s="45">
-        <v>0</v>
-      </c>
-      <c r="K16" s="46">
-        <v>1</v>
-      </c>
-      <c r="L16" s="46" t="s">
+      <c r="J16" s="211">
+        <v>1</v>
+      </c>
+      <c r="K16" s="45">
+        <v>0</v>
+      </c>
+      <c r="L16" s="46">
+        <v>1</v>
+      </c>
+      <c r="M16" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="M16" s="46">
-        <v>0</v>
-      </c>
       <c r="N16" s="46">
         <v>0</v>
       </c>
-      <c r="O16" s="47">
-        <v>1</v>
-      </c>
-      <c r="P16" s="48">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="49">
-        <v>0</v>
-      </c>
-      <c r="R16" s="199" t="s">
+      <c r="O16" s="46">
+        <v>0</v>
+      </c>
+      <c r="P16" s="47">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="48">
+        <v>0</v>
+      </c>
+      <c r="R16" s="49">
+        <v>0</v>
+      </c>
+      <c r="S16" s="199" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="50" t="s">
         <v>44</v>
       </c>
@@ -2187,35 +2250,38 @@
       <c r="I17" s="44">
         <v>1</v>
       </c>
-      <c r="J17" s="45">
-        <v>0</v>
-      </c>
-      <c r="K17" s="46">
-        <v>1</v>
-      </c>
-      <c r="L17" s="46" t="s">
+      <c r="J17" s="211">
+        <v>1</v>
+      </c>
+      <c r="K17" s="45">
+        <v>0</v>
+      </c>
+      <c r="L17" s="46">
+        <v>1</v>
+      </c>
+      <c r="M17" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="M17" s="46">
-        <v>0</v>
-      </c>
       <c r="N17" s="46">
         <v>0</v>
       </c>
-      <c r="O17" s="47">
-        <v>0</v>
-      </c>
-      <c r="P17" s="48">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="49">
-        <v>0</v>
-      </c>
-      <c r="R17" s="199" t="s">
+      <c r="O17" s="46">
+        <v>0</v>
+      </c>
+      <c r="P17" s="47">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="48">
+        <v>0</v>
+      </c>
+      <c r="R17" s="49">
+        <v>0</v>
+      </c>
+      <c r="S17" s="199" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="51" t="s">
         <v>45</v>
       </c>
@@ -2243,35 +2309,38 @@
       <c r="I18" s="53">
         <v>1</v>
       </c>
-      <c r="J18" s="54">
-        <v>0</v>
-      </c>
-      <c r="K18" s="55">
-        <v>1</v>
-      </c>
-      <c r="L18" s="55" t="s">
+      <c r="J18" s="212">
+        <v>1</v>
+      </c>
+      <c r="K18" s="54">
+        <v>0</v>
+      </c>
+      <c r="L18" s="55">
+        <v>1</v>
+      </c>
+      <c r="M18" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="M18" s="55">
-        <v>0</v>
-      </c>
       <c r="N18" s="55">
         <v>0</v>
       </c>
-      <c r="O18" s="56">
-        <v>1</v>
-      </c>
-      <c r="P18" s="57">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="58">
-        <v>0</v>
-      </c>
-      <c r="R18" s="199" t="s">
+      <c r="O18" s="55">
+        <v>0</v>
+      </c>
+      <c r="P18" s="56">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="57">
+        <v>0</v>
+      </c>
+      <c r="R18" s="58">
+        <v>0</v>
+      </c>
+      <c r="S18" s="199" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="10"/>
       <c r="C19" s="5"/>
@@ -2281,28 +2350,29 @@
       <c r="G19" s="6"/>
       <c r="H19" s="133"/>
       <c r="I19" s="6"/>
-      <c r="J19" s="11">
-        <v>0</v>
-      </c>
-      <c r="K19" s="12">
-        <v>1</v>
-      </c>
-      <c r="L19" s="12" t="s">
+      <c r="J19" s="7"/>
+      <c r="K19" s="11">
+        <v>0</v>
+      </c>
+      <c r="L19" s="12">
+        <v>1</v>
+      </c>
+      <c r="M19" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="M19" s="12">
-        <v>1</v>
-      </c>
       <c r="N19" s="12">
         <v>1</v>
       </c>
-      <c r="O19" s="13">
-        <v>1</v>
-      </c>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="7"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="O19" s="12">
+        <v>1</v>
+      </c>
+      <c r="P19" s="13">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="7"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="60" t="s">
         <v>10</v>
       </c>
@@ -2330,35 +2400,38 @@
       <c r="I20" s="62">
         <v>0</v>
       </c>
-      <c r="J20" s="63">
-        <v>1</v>
-      </c>
-      <c r="K20" s="64">
-        <v>0</v>
-      </c>
-      <c r="L20" s="64" t="s">
+      <c r="J20" s="213">
+        <v>1</v>
+      </c>
+      <c r="K20" s="63">
+        <v>1</v>
+      </c>
+      <c r="L20" s="64">
+        <v>0</v>
+      </c>
+      <c r="M20" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="M20" s="64">
-        <v>0</v>
-      </c>
       <c r="N20" s="64">
         <v>0</v>
       </c>
-      <c r="O20" s="65">
-        <v>0</v>
-      </c>
-      <c r="P20" s="66">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="67">
-        <v>0</v>
-      </c>
-      <c r="R20" s="200" t="s">
+      <c r="O20" s="64">
+        <v>0</v>
+      </c>
+      <c r="P20" s="65">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="66">
+        <v>0</v>
+      </c>
+      <c r="R20" s="67">
+        <v>0</v>
+      </c>
+      <c r="S20" s="200" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="60" t="s">
         <v>11</v>
       </c>
@@ -2386,35 +2459,38 @@
       <c r="I21" s="62">
         <v>0</v>
       </c>
-      <c r="J21" s="63">
-        <v>1</v>
-      </c>
-      <c r="K21" s="64">
-        <v>0</v>
-      </c>
-      <c r="L21" s="64" t="s">
+      <c r="J21" s="213">
+        <v>1</v>
+      </c>
+      <c r="K21" s="63">
+        <v>1</v>
+      </c>
+      <c r="L21" s="64">
+        <v>0</v>
+      </c>
+      <c r="M21" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="M21" s="64">
-        <v>0</v>
-      </c>
       <c r="N21" s="64">
         <v>0</v>
       </c>
-      <c r="O21" s="65">
-        <v>1</v>
-      </c>
-      <c r="P21" s="66">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="67">
-        <v>0</v>
-      </c>
-      <c r="R21" s="200" t="s">
+      <c r="O21" s="64">
+        <v>0</v>
+      </c>
+      <c r="P21" s="65">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="66">
+        <v>0</v>
+      </c>
+      <c r="R21" s="67">
+        <v>0</v>
+      </c>
+      <c r="S21" s="200" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="60" t="s">
         <v>12</v>
       </c>
@@ -2442,35 +2518,38 @@
       <c r="I22" s="62">
         <v>0</v>
       </c>
-      <c r="J22" s="63">
-        <v>1</v>
-      </c>
-      <c r="K22" s="64">
-        <v>0</v>
-      </c>
-      <c r="L22" s="64" t="s">
+      <c r="J22" s="213">
+        <v>1</v>
+      </c>
+      <c r="K22" s="63">
+        <v>1</v>
+      </c>
+      <c r="L22" s="64">
+        <v>0</v>
+      </c>
+      <c r="M22" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="M22" s="64">
-        <v>0</v>
-      </c>
       <c r="N22" s="64">
-        <v>1</v>
-      </c>
-      <c r="O22" s="65">
-        <v>0</v>
-      </c>
-      <c r="P22" s="66">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="67">
-        <v>0</v>
-      </c>
-      <c r="R22" s="200" t="s">
+        <v>0</v>
+      </c>
+      <c r="O22" s="64">
+        <v>1</v>
+      </c>
+      <c r="P22" s="65">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="66">
+        <v>0</v>
+      </c>
+      <c r="R22" s="67">
+        <v>0</v>
+      </c>
+      <c r="S22" s="200" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="68" t="s">
         <v>13</v>
       </c>
@@ -2498,35 +2577,38 @@
       <c r="I23" s="70">
         <v>0</v>
       </c>
-      <c r="J23" s="71">
-        <v>1</v>
-      </c>
-      <c r="K23" s="72">
-        <v>0</v>
-      </c>
-      <c r="L23" s="72" t="s">
+      <c r="J23" s="214">
+        <v>1</v>
+      </c>
+      <c r="K23" s="71">
+        <v>1</v>
+      </c>
+      <c r="L23" s="72">
+        <v>0</v>
+      </c>
+      <c r="M23" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="M23" s="72">
-        <v>0</v>
-      </c>
       <c r="N23" s="72">
-        <v>1</v>
-      </c>
-      <c r="O23" s="73">
-        <v>1</v>
-      </c>
-      <c r="P23" s="74">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="75">
-        <v>0</v>
-      </c>
-      <c r="R23" s="200" t="s">
+        <v>0</v>
+      </c>
+      <c r="O23" s="72">
+        <v>1</v>
+      </c>
+      <c r="P23" s="73">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="74">
+        <v>0</v>
+      </c>
+      <c r="R23" s="75">
+        <v>0</v>
+      </c>
+      <c r="S23" s="200" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="60" t="s">
         <v>30</v>
       </c>
@@ -2554,35 +2636,38 @@
       <c r="I24" s="62">
         <v>1</v>
       </c>
-      <c r="J24" s="63">
-        <v>1</v>
-      </c>
-      <c r="K24" s="64">
-        <v>0</v>
-      </c>
-      <c r="L24" s="64" t="s">
+      <c r="J24" s="213">
+        <v>1</v>
+      </c>
+      <c r="K24" s="63">
+        <v>1</v>
+      </c>
+      <c r="L24" s="64">
+        <v>0</v>
+      </c>
+      <c r="M24" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="M24" s="64">
-        <v>0</v>
-      </c>
       <c r="N24" s="64">
         <v>0</v>
       </c>
-      <c r="O24" s="65">
-        <v>0</v>
-      </c>
-      <c r="P24" s="66">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="67">
-        <v>0</v>
-      </c>
-      <c r="R24" s="200" t="s">
+      <c r="O24" s="64">
+        <v>0</v>
+      </c>
+      <c r="P24" s="65">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="66">
+        <v>0</v>
+      </c>
+      <c r="R24" s="67">
+        <v>0</v>
+      </c>
+      <c r="S24" s="200" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="60" t="s">
         <v>31</v>
       </c>
@@ -2610,35 +2695,38 @@
       <c r="I25" s="62">
         <v>1</v>
       </c>
-      <c r="J25" s="63">
-        <v>1</v>
-      </c>
-      <c r="K25" s="64">
-        <v>0</v>
-      </c>
-      <c r="L25" s="64" t="s">
+      <c r="J25" s="213">
+        <v>1</v>
+      </c>
+      <c r="K25" s="63">
+        <v>1</v>
+      </c>
+      <c r="L25" s="64">
+        <v>0</v>
+      </c>
+      <c r="M25" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="M25" s="64">
-        <v>0</v>
-      </c>
       <c r="N25" s="64">
         <v>0</v>
       </c>
-      <c r="O25" s="65">
-        <v>1</v>
-      </c>
-      <c r="P25" s="66">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="67">
-        <v>0</v>
-      </c>
-      <c r="R25" s="200" t="s">
+      <c r="O25" s="64">
+        <v>0</v>
+      </c>
+      <c r="P25" s="65">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="66">
+        <v>0</v>
+      </c>
+      <c r="R25" s="67">
+        <v>0</v>
+      </c>
+      <c r="S25" s="200" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="60" t="s">
         <v>32</v>
       </c>
@@ -2666,35 +2754,38 @@
       <c r="I26" s="62">
         <v>1</v>
       </c>
-      <c r="J26" s="63">
-        <v>1</v>
-      </c>
-      <c r="K26" s="64">
-        <v>0</v>
-      </c>
-      <c r="L26" s="64" t="s">
+      <c r="J26" s="213">
+        <v>1</v>
+      </c>
+      <c r="K26" s="63">
+        <v>1</v>
+      </c>
+      <c r="L26" s="64">
+        <v>0</v>
+      </c>
+      <c r="M26" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="M26" s="64">
-        <v>0</v>
-      </c>
       <c r="N26" s="64">
-        <v>1</v>
-      </c>
-      <c r="O26" s="65">
-        <v>0</v>
-      </c>
-      <c r="P26" s="66">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="67">
-        <v>0</v>
-      </c>
-      <c r="R26" s="200" t="s">
+        <v>0</v>
+      </c>
+      <c r="O26" s="64">
+        <v>1</v>
+      </c>
+      <c r="P26" s="65">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="66">
+        <v>0</v>
+      </c>
+      <c r="R26" s="67">
+        <v>0</v>
+      </c>
+      <c r="S26" s="200" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="68" t="s">
         <v>33</v>
       </c>
@@ -2722,35 +2813,38 @@
       <c r="I27" s="70">
         <v>1</v>
       </c>
-      <c r="J27" s="71">
-        <v>1</v>
-      </c>
-      <c r="K27" s="72">
-        <v>0</v>
-      </c>
-      <c r="L27" s="72" t="s">
+      <c r="J27" s="214">
+        <v>1</v>
+      </c>
+      <c r="K27" s="71">
+        <v>1</v>
+      </c>
+      <c r="L27" s="72">
+        <v>0</v>
+      </c>
+      <c r="M27" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="M27" s="72">
-        <v>0</v>
-      </c>
       <c r="N27" s="72">
-        <v>1</v>
-      </c>
-      <c r="O27" s="73">
-        <v>1</v>
-      </c>
-      <c r="P27" s="74">
-        <v>0</v>
-      </c>
-      <c r="Q27" s="75">
-        <v>0</v>
-      </c>
-      <c r="R27" s="200" t="s">
+        <v>0</v>
+      </c>
+      <c r="O27" s="72">
+        <v>1</v>
+      </c>
+      <c r="P27" s="73">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="74">
+        <v>0</v>
+      </c>
+      <c r="R27" s="75">
+        <v>0</v>
+      </c>
+      <c r="S27" s="200" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="10"/>
       <c r="C28" s="5"/>
@@ -2760,16 +2854,17 @@
       <c r="G28" s="6"/>
       <c r="H28" s="133"/>
       <c r="I28" s="6"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="12"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="11"/>
       <c r="L28" s="12"/>
       <c r="M28" s="12"/>
       <c r="N28" s="12"/>
-      <c r="O28" s="13"/>
-      <c r="P28" s="6"/>
-      <c r="Q28" s="7"/>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="O28" s="12"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="7"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="77" t="s">
         <v>35</v>
       </c>
@@ -2797,35 +2892,38 @@
       <c r="I29" s="79">
         <v>0</v>
       </c>
-      <c r="J29" s="80">
-        <v>1</v>
-      </c>
-      <c r="K29" s="81">
-        <v>1</v>
-      </c>
-      <c r="L29" s="81" t="s">
+      <c r="J29" s="215">
+        <v>1</v>
+      </c>
+      <c r="K29" s="80">
+        <v>1</v>
+      </c>
+      <c r="L29" s="81">
+        <v>1</v>
+      </c>
+      <c r="M29" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="M29" s="81">
-        <v>0</v>
-      </c>
       <c r="N29" s="81">
         <v>0</v>
       </c>
-      <c r="O29" s="82">
-        <v>0</v>
-      </c>
-      <c r="P29" s="83">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="84">
-        <v>0</v>
-      </c>
-      <c r="R29" s="201" t="s">
+      <c r="O29" s="81">
+        <v>0</v>
+      </c>
+      <c r="P29" s="82">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="83">
+        <v>0</v>
+      </c>
+      <c r="R29" s="84">
+        <v>0</v>
+      </c>
+      <c r="S29" s="201" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="77" t="s">
         <v>34</v>
       </c>
@@ -2853,35 +2951,38 @@
       <c r="I30" s="79">
         <v>0</v>
       </c>
-      <c r="J30" s="80">
-        <v>1</v>
-      </c>
-      <c r="K30" s="81">
-        <v>1</v>
-      </c>
-      <c r="L30" s="81" t="s">
+      <c r="J30" s="215">
+        <v>1</v>
+      </c>
+      <c r="K30" s="80">
+        <v>1</v>
+      </c>
+      <c r="L30" s="81">
+        <v>1</v>
+      </c>
+      <c r="M30" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="M30" s="81">
-        <v>0</v>
-      </c>
       <c r="N30" s="81">
         <v>0</v>
       </c>
-      <c r="O30" s="82">
-        <v>1</v>
-      </c>
-      <c r="P30" s="83">
-        <v>0</v>
-      </c>
-      <c r="Q30" s="84">
-        <v>0</v>
-      </c>
-      <c r="R30" s="201" t="s">
+      <c r="O30" s="81">
+        <v>0</v>
+      </c>
+      <c r="P30" s="82">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="83">
+        <v>0</v>
+      </c>
+      <c r="R30" s="84">
+        <v>0</v>
+      </c>
+      <c r="S30" s="201" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="77" t="s">
         <v>36</v>
       </c>
@@ -2909,35 +3010,38 @@
       <c r="I31" s="79">
         <v>0</v>
       </c>
-      <c r="J31" s="80">
-        <v>1</v>
-      </c>
-      <c r="K31" s="81">
-        <v>1</v>
-      </c>
-      <c r="L31" s="81" t="s">
+      <c r="J31" s="215">
+        <v>1</v>
+      </c>
+      <c r="K31" s="80">
+        <v>1</v>
+      </c>
+      <c r="L31" s="81">
+        <v>1</v>
+      </c>
+      <c r="M31" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="M31" s="81">
-        <v>0</v>
-      </c>
       <c r="N31" s="81">
-        <v>1</v>
-      </c>
-      <c r="O31" s="82">
-        <v>0</v>
-      </c>
-      <c r="P31" s="83">
-        <v>0</v>
-      </c>
-      <c r="Q31" s="84">
-        <v>0</v>
-      </c>
-      <c r="R31" s="201" t="s">
+        <v>0</v>
+      </c>
+      <c r="O31" s="81">
+        <v>1</v>
+      </c>
+      <c r="P31" s="82">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="83">
+        <v>0</v>
+      </c>
+      <c r="R31" s="84">
+        <v>0</v>
+      </c>
+      <c r="S31" s="201" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="77" t="s">
         <v>14</v>
       </c>
@@ -2965,35 +3069,38 @@
       <c r="I32" s="79">
         <v>0</v>
       </c>
-      <c r="J32" s="80">
-        <v>1</v>
-      </c>
-      <c r="K32" s="81">
-        <v>1</v>
-      </c>
-      <c r="L32" s="81" t="s">
+      <c r="J32" s="215">
+        <v>1</v>
+      </c>
+      <c r="K32" s="80">
+        <v>1</v>
+      </c>
+      <c r="L32" s="81">
+        <v>1</v>
+      </c>
+      <c r="M32" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="M32" s="81">
-        <v>0</v>
-      </c>
       <c r="N32" s="81">
-        <v>1</v>
-      </c>
-      <c r="O32" s="82">
-        <v>1</v>
-      </c>
-      <c r="P32" s="83">
-        <v>0</v>
-      </c>
-      <c r="Q32" s="84">
-        <v>0</v>
-      </c>
-      <c r="R32" s="201" t="s">
+        <v>0</v>
+      </c>
+      <c r="O32" s="81">
+        <v>1</v>
+      </c>
+      <c r="P32" s="82">
+        <v>1</v>
+      </c>
+      <c r="Q32" s="83">
+        <v>0</v>
+      </c>
+      <c r="R32" s="84">
+        <v>0</v>
+      </c>
+      <c r="S32" s="201" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" s="77" t="s">
         <v>37</v>
       </c>
@@ -3021,35 +3128,38 @@
       <c r="I33" s="79">
         <v>0</v>
       </c>
-      <c r="J33" s="80">
-        <v>1</v>
-      </c>
-      <c r="K33" s="81">
-        <v>1</v>
-      </c>
-      <c r="L33" s="81" t="s">
+      <c r="J33" s="215">
+        <v>1</v>
+      </c>
+      <c r="K33" s="80">
+        <v>1</v>
+      </c>
+      <c r="L33" s="81">
+        <v>1</v>
+      </c>
+      <c r="M33" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="M33" s="81">
-        <v>1</v>
-      </c>
       <c r="N33" s="81">
-        <v>0</v>
-      </c>
-      <c r="O33" s="82">
-        <v>0</v>
-      </c>
-      <c r="P33" s="83">
-        <v>0</v>
-      </c>
-      <c r="Q33" s="84">
-        <v>0</v>
-      </c>
-      <c r="R33" s="201" t="s">
+        <v>1</v>
+      </c>
+      <c r="O33" s="81">
+        <v>0</v>
+      </c>
+      <c r="P33" s="82">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="83">
+        <v>0</v>
+      </c>
+      <c r="R33" s="84">
+        <v>0</v>
+      </c>
+      <c r="S33" s="201" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" s="77" t="s">
         <v>15</v>
       </c>
@@ -3077,35 +3187,38 @@
       <c r="I34" s="79">
         <v>0</v>
       </c>
-      <c r="J34" s="80">
-        <v>1</v>
-      </c>
-      <c r="K34" s="81">
-        <v>1</v>
-      </c>
-      <c r="L34" s="81" t="s">
+      <c r="J34" s="215">
+        <v>1</v>
+      </c>
+      <c r="K34" s="80">
+        <v>1</v>
+      </c>
+      <c r="L34" s="81">
+        <v>1</v>
+      </c>
+      <c r="M34" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="M34" s="81">
-        <v>1</v>
-      </c>
       <c r="N34" s="81">
-        <v>0</v>
-      </c>
-      <c r="O34" s="82">
-        <v>1</v>
-      </c>
-      <c r="P34" s="83">
-        <v>0</v>
-      </c>
-      <c r="Q34" s="84">
-        <v>0</v>
-      </c>
-      <c r="R34" s="201" t="s">
+        <v>1</v>
+      </c>
+      <c r="O34" s="81">
+        <v>0</v>
+      </c>
+      <c r="P34" s="82">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="83">
+        <v>0</v>
+      </c>
+      <c r="R34" s="84">
+        <v>0</v>
+      </c>
+      <c r="S34" s="201" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" s="85" t="s">
         <v>38</v>
       </c>
@@ -3133,35 +3246,38 @@
       <c r="I35" s="87">
         <v>0</v>
       </c>
-      <c r="J35" s="88">
-        <v>1</v>
-      </c>
-      <c r="K35" s="89">
-        <v>1</v>
-      </c>
-      <c r="L35" s="89" t="s">
+      <c r="J35" s="216">
+        <v>1</v>
+      </c>
+      <c r="K35" s="88">
+        <v>1</v>
+      </c>
+      <c r="L35" s="89">
+        <v>1</v>
+      </c>
+      <c r="M35" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="M35" s="89">
-        <v>1</v>
-      </c>
       <c r="N35" s="89">
         <v>1</v>
       </c>
-      <c r="O35" s="90">
-        <v>0</v>
-      </c>
-      <c r="P35" s="91">
-        <v>0</v>
-      </c>
-      <c r="Q35" s="92">
-        <v>0</v>
-      </c>
-      <c r="R35" s="201" t="s">
+      <c r="O35" s="89">
+        <v>1</v>
+      </c>
+      <c r="P35" s="90">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="91">
+        <v>0</v>
+      </c>
+      <c r="R35" s="92">
+        <v>0</v>
+      </c>
+      <c r="S35" s="201" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36" s="77" t="s">
         <v>46</v>
       </c>
@@ -3189,35 +3305,38 @@
       <c r="I36" s="79">
         <v>1</v>
       </c>
-      <c r="J36" s="80">
-        <v>1</v>
-      </c>
-      <c r="K36" s="81">
-        <v>1</v>
-      </c>
-      <c r="L36" s="81" t="s">
+      <c r="J36" s="215">
+        <v>1</v>
+      </c>
+      <c r="K36" s="80">
+        <v>1</v>
+      </c>
+      <c r="L36" s="81">
+        <v>1</v>
+      </c>
+      <c r="M36" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="M36" s="81">
-        <v>0</v>
-      </c>
       <c r="N36" s="81">
         <v>0</v>
       </c>
-      <c r="O36" s="82">
-        <v>0</v>
-      </c>
-      <c r="P36" s="83">
-        <v>0</v>
-      </c>
-      <c r="Q36" s="84">
-        <v>0</v>
-      </c>
-      <c r="R36" s="201" t="s">
+      <c r="O36" s="81">
+        <v>0</v>
+      </c>
+      <c r="P36" s="82">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="83">
+        <v>0</v>
+      </c>
+      <c r="R36" s="84">
+        <v>0</v>
+      </c>
+      <c r="S36" s="201" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37" s="77" t="s">
         <v>47</v>
       </c>
@@ -3245,35 +3364,38 @@
       <c r="I37" s="79">
         <v>1</v>
       </c>
-      <c r="J37" s="80">
-        <v>1</v>
-      </c>
-      <c r="K37" s="81">
-        <v>1</v>
-      </c>
-      <c r="L37" s="81" t="s">
+      <c r="J37" s="215">
+        <v>1</v>
+      </c>
+      <c r="K37" s="80">
+        <v>1</v>
+      </c>
+      <c r="L37" s="81">
+        <v>1</v>
+      </c>
+      <c r="M37" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="M37" s="81">
-        <v>0</v>
-      </c>
       <c r="N37" s="81">
         <v>0</v>
       </c>
-      <c r="O37" s="82">
-        <v>1</v>
-      </c>
-      <c r="P37" s="83">
-        <v>0</v>
-      </c>
-      <c r="Q37" s="84">
-        <v>0</v>
-      </c>
-      <c r="R37" s="201" t="s">
+      <c r="O37" s="81">
+        <v>0</v>
+      </c>
+      <c r="P37" s="82">
+        <v>1</v>
+      </c>
+      <c r="Q37" s="83">
+        <v>0</v>
+      </c>
+      <c r="R37" s="84">
+        <v>0</v>
+      </c>
+      <c r="S37" s="201" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38" s="77" t="s">
         <v>48</v>
       </c>
@@ -3301,35 +3423,38 @@
       <c r="I38" s="79">
         <v>1</v>
       </c>
-      <c r="J38" s="80">
-        <v>1</v>
-      </c>
-      <c r="K38" s="81">
-        <v>1</v>
-      </c>
-      <c r="L38" s="81" t="s">
+      <c r="J38" s="215">
+        <v>1</v>
+      </c>
+      <c r="K38" s="80">
+        <v>1</v>
+      </c>
+      <c r="L38" s="81">
+        <v>1</v>
+      </c>
+      <c r="M38" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="M38" s="81">
-        <v>0</v>
-      </c>
       <c r="N38" s="81">
-        <v>1</v>
-      </c>
-      <c r="O38" s="82">
-        <v>0</v>
-      </c>
-      <c r="P38" s="83">
-        <v>0</v>
-      </c>
-      <c r="Q38" s="84">
-        <v>0</v>
-      </c>
-      <c r="R38" s="201" t="s">
+        <v>0</v>
+      </c>
+      <c r="O38" s="81">
+        <v>1</v>
+      </c>
+      <c r="P38" s="82">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="83">
+        <v>0</v>
+      </c>
+      <c r="R38" s="84">
+        <v>0</v>
+      </c>
+      <c r="S38" s="201" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39" s="77" t="s">
         <v>49</v>
       </c>
@@ -3357,35 +3482,38 @@
       <c r="I39" s="79">
         <v>1</v>
       </c>
-      <c r="J39" s="80">
-        <v>1</v>
-      </c>
-      <c r="K39" s="81">
-        <v>1</v>
-      </c>
-      <c r="L39" s="81" t="s">
+      <c r="J39" s="215">
+        <v>1</v>
+      </c>
+      <c r="K39" s="80">
+        <v>1</v>
+      </c>
+      <c r="L39" s="81">
+        <v>1</v>
+      </c>
+      <c r="M39" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="81">
-        <v>0</v>
-      </c>
       <c r="N39" s="81">
-        <v>1</v>
-      </c>
-      <c r="O39" s="82">
-        <v>1</v>
-      </c>
-      <c r="P39" s="83">
-        <v>0</v>
-      </c>
-      <c r="Q39" s="84">
-        <v>0</v>
-      </c>
-      <c r="R39" s="201" t="s">
+        <v>0</v>
+      </c>
+      <c r="O39" s="81">
+        <v>1</v>
+      </c>
+      <c r="P39" s="82">
+        <v>1</v>
+      </c>
+      <c r="Q39" s="83">
+        <v>0</v>
+      </c>
+      <c r="R39" s="84">
+        <v>0</v>
+      </c>
+      <c r="S39" s="201" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A40" s="77" t="s">
         <v>50</v>
       </c>
@@ -3413,35 +3541,38 @@
       <c r="I40" s="79">
         <v>1</v>
       </c>
-      <c r="J40" s="80">
-        <v>1</v>
-      </c>
-      <c r="K40" s="81">
-        <v>1</v>
-      </c>
-      <c r="L40" s="81" t="s">
+      <c r="J40" s="215">
+        <v>1</v>
+      </c>
+      <c r="K40" s="80">
+        <v>1</v>
+      </c>
+      <c r="L40" s="81">
+        <v>1</v>
+      </c>
+      <c r="M40" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="M40" s="81">
-        <v>1</v>
-      </c>
       <c r="N40" s="81">
-        <v>0</v>
-      </c>
-      <c r="O40" s="82">
-        <v>0</v>
-      </c>
-      <c r="P40" s="83">
-        <v>0</v>
-      </c>
-      <c r="Q40" s="84">
-        <v>0</v>
-      </c>
-      <c r="R40" s="201" t="s">
+        <v>1</v>
+      </c>
+      <c r="O40" s="81">
+        <v>0</v>
+      </c>
+      <c r="P40" s="82">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="83">
+        <v>0</v>
+      </c>
+      <c r="R40" s="84">
+        <v>0</v>
+      </c>
+      <c r="S40" s="201" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A41" s="77" t="s">
         <v>51</v>
       </c>
@@ -3469,35 +3600,38 @@
       <c r="I41" s="79">
         <v>1</v>
       </c>
-      <c r="J41" s="80">
-        <v>1</v>
-      </c>
-      <c r="K41" s="81">
-        <v>1</v>
-      </c>
-      <c r="L41" s="81" t="s">
+      <c r="J41" s="215">
+        <v>1</v>
+      </c>
+      <c r="K41" s="80">
+        <v>1</v>
+      </c>
+      <c r="L41" s="81">
+        <v>1</v>
+      </c>
+      <c r="M41" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="M41" s="81">
-        <v>1</v>
-      </c>
       <c r="N41" s="81">
-        <v>0</v>
-      </c>
-      <c r="O41" s="82">
-        <v>1</v>
-      </c>
-      <c r="P41" s="83">
-        <v>0</v>
-      </c>
-      <c r="Q41" s="84">
-        <v>0</v>
-      </c>
-      <c r="R41" s="201" t="s">
+        <v>1</v>
+      </c>
+      <c r="O41" s="81">
+        <v>0</v>
+      </c>
+      <c r="P41" s="82">
+        <v>1</v>
+      </c>
+      <c r="Q41" s="83">
+        <v>0</v>
+      </c>
+      <c r="R41" s="84">
+        <v>0</v>
+      </c>
+      <c r="S41" s="201" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A42" s="85" t="s">
         <v>52</v>
       </c>
@@ -3525,35 +3659,38 @@
       <c r="I42" s="87">
         <v>1</v>
       </c>
-      <c r="J42" s="88">
-        <v>1</v>
-      </c>
-      <c r="K42" s="89">
-        <v>1</v>
-      </c>
-      <c r="L42" s="89" t="s">
+      <c r="J42" s="216">
+        <v>1</v>
+      </c>
+      <c r="K42" s="88">
+        <v>1</v>
+      </c>
+      <c r="L42" s="89">
+        <v>1</v>
+      </c>
+      <c r="M42" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="M42" s="89">
-        <v>1</v>
-      </c>
       <c r="N42" s="89">
         <v>1</v>
       </c>
-      <c r="O42" s="90">
-        <v>0</v>
-      </c>
-      <c r="P42" s="91">
-        <v>0</v>
-      </c>
-      <c r="Q42" s="92">
-        <v>0</v>
-      </c>
-      <c r="R42" s="201" t="s">
+      <c r="O42" s="89">
+        <v>1</v>
+      </c>
+      <c r="P42" s="90">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="91">
+        <v>0</v>
+      </c>
+      <c r="R42" s="92">
+        <v>0</v>
+      </c>
+      <c r="S42" s="201" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="10"/>
       <c r="C43" s="5"/>
@@ -3563,16 +3700,17 @@
       <c r="G43" s="6"/>
       <c r="H43" s="133"/>
       <c r="I43" s="6"/>
-      <c r="J43" s="11"/>
-      <c r="K43" s="12"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="11"/>
       <c r="L43" s="12"/>
       <c r="M43" s="12"/>
       <c r="N43" s="12"/>
-      <c r="O43" s="13"/>
-      <c r="P43" s="8"/>
-      <c r="Q43" s="9"/>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="O43" s="12"/>
+      <c r="P43" s="13"/>
+      <c r="Q43" s="8"/>
+      <c r="R43" s="9"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A44" s="121" t="s">
         <v>16</v>
       </c>
@@ -3600,35 +3738,38 @@
       <c r="I44" s="123">
         <v>0</v>
       </c>
-      <c r="J44" s="124">
-        <v>1</v>
-      </c>
-      <c r="K44" s="125">
-        <v>1</v>
-      </c>
-      <c r="L44" s="126">
-        <v>1</v>
-      </c>
-      <c r="M44" s="125">
+      <c r="J44" s="217">
+        <v>1</v>
+      </c>
+      <c r="K44" s="124">
+        <v>1</v>
+      </c>
+      <c r="L44" s="125">
+        <v>1</v>
+      </c>
+      <c r="M44" s="126">
         <v>1</v>
       </c>
       <c r="N44" s="125">
         <v>1</v>
       </c>
-      <c r="O44" s="127">
-        <v>1</v>
-      </c>
-      <c r="P44" s="128">
-        <v>0</v>
-      </c>
-      <c r="Q44" s="129">
-        <v>0</v>
-      </c>
-      <c r="R44" s="206" t="s">
+      <c r="O44" s="125">
+        <v>1</v>
+      </c>
+      <c r="P44" s="127">
+        <v>1</v>
+      </c>
+      <c r="Q44" s="128">
+        <v>0</v>
+      </c>
+      <c r="R44" s="129">
+        <v>0</v>
+      </c>
+      <c r="S44" s="206" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A45" s="94" t="s">
         <v>60</v>
       </c>
@@ -3656,35 +3797,38 @@
       <c r="I45" s="96">
         <v>1</v>
       </c>
-      <c r="J45" s="97">
-        <v>1</v>
-      </c>
-      <c r="K45" s="98">
-        <v>1</v>
-      </c>
-      <c r="L45" s="99">
-        <v>1</v>
-      </c>
-      <c r="M45" s="98">
+      <c r="J45" s="218">
+        <v>1</v>
+      </c>
+      <c r="K45" s="97">
+        <v>1</v>
+      </c>
+      <c r="L45" s="98">
+        <v>1</v>
+      </c>
+      <c r="M45" s="99">
         <v>1</v>
       </c>
       <c r="N45" s="98">
         <v>1</v>
       </c>
-      <c r="O45" s="100">
-        <v>1</v>
-      </c>
-      <c r="P45" s="101">
-        <v>0</v>
-      </c>
-      <c r="Q45" s="102">
-        <v>0</v>
-      </c>
-      <c r="R45" s="206" t="s">
+      <c r="O45" s="98">
+        <v>1</v>
+      </c>
+      <c r="P45" s="100">
+        <v>1</v>
+      </c>
+      <c r="Q45" s="101">
+        <v>0</v>
+      </c>
+      <c r="R45" s="102">
+        <v>0</v>
+      </c>
+      <c r="S45" s="206" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
       <c r="B46" s="10"/>
       <c r="C46" s="5"/>
@@ -3694,16 +3838,17 @@
       <c r="G46" s="6"/>
       <c r="H46" s="133"/>
       <c r="I46" s="6"/>
-      <c r="J46" s="14"/>
-      <c r="K46" s="15"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="14"/>
       <c r="L46" s="15"/>
       <c r="M46" s="15"/>
       <c r="N46" s="15"/>
-      <c r="O46" s="16"/>
-      <c r="P46" s="6"/>
-      <c r="Q46" s="7"/>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="O46" s="15"/>
+      <c r="P46" s="16"/>
+      <c r="Q46" s="6"/>
+      <c r="R46" s="7"/>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A47" s="104" t="s">
         <v>39</v>
       </c>
@@ -3731,35 +3876,38 @@
       <c r="I47" s="106">
         <v>1</v>
       </c>
-      <c r="J47" s="107">
-        <v>0</v>
-      </c>
-      <c r="K47" s="108">
-        <v>1</v>
-      </c>
-      <c r="L47" s="108" t="s">
+      <c r="J47" s="219">
+        <v>1</v>
+      </c>
+      <c r="K47" s="107">
+        <v>0</v>
+      </c>
+      <c r="L47" s="108">
+        <v>1</v>
+      </c>
+      <c r="M47" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="M47" s="108">
-        <v>0</v>
-      </c>
       <c r="N47" s="108">
         <v>0</v>
       </c>
-      <c r="O47" s="109">
-        <v>0</v>
-      </c>
-      <c r="P47" s="110">
-        <v>0</v>
-      </c>
-      <c r="Q47" s="111">
-        <v>1</v>
-      </c>
-      <c r="R47" s="203" t="s">
+      <c r="O47" s="108">
+        <v>0</v>
+      </c>
+      <c r="P47" s="109">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="110">
+        <v>0</v>
+      </c>
+      <c r="R47" s="111">
+        <v>1</v>
+      </c>
+      <c r="S47" s="203" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A48" s="112" t="s">
         <v>40</v>
       </c>
@@ -3787,35 +3935,38 @@
       <c r="I48" s="114">
         <v>1</v>
       </c>
-      <c r="J48" s="115">
-        <v>0</v>
-      </c>
-      <c r="K48" s="116">
-        <v>1</v>
-      </c>
-      <c r="L48" s="116" t="s">
+      <c r="J48" s="220">
+        <v>1</v>
+      </c>
+      <c r="K48" s="115">
+        <v>0</v>
+      </c>
+      <c r="L48" s="116">
+        <v>1</v>
+      </c>
+      <c r="M48" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="M48" s="116">
-        <v>0</v>
-      </c>
       <c r="N48" s="116">
         <v>0</v>
       </c>
-      <c r="O48" s="117">
-        <v>0</v>
-      </c>
-      <c r="P48" s="118">
-        <v>1</v>
-      </c>
-      <c r="Q48" s="119">
-        <v>0</v>
-      </c>
-      <c r="R48" s="203" t="s">
+      <c r="O48" s="116">
+        <v>0</v>
+      </c>
+      <c r="P48" s="117">
+        <v>0</v>
+      </c>
+      <c r="Q48" s="118">
+        <v>1</v>
+      </c>
+      <c r="R48" s="119">
+        <v>0</v>
+      </c>
+      <c r="S48" s="203" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A49" s="3"/>
       <c r="B49" s="10"/>
       <c r="C49" s="5"/>
@@ -3825,16 +3976,17 @@
       <c r="G49" s="6"/>
       <c r="H49" s="133"/>
       <c r="I49" s="6"/>
-      <c r="J49" s="17"/>
-      <c r="K49" s="18"/>
+      <c r="J49" s="7"/>
+      <c r="K49" s="17"/>
       <c r="L49" s="18"/>
       <c r="M49" s="18"/>
       <c r="N49" s="18"/>
-      <c r="O49" s="19"/>
-      <c r="P49" s="6"/>
-      <c r="Q49" s="7"/>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="O49" s="18"/>
+      <c r="P49" s="19"/>
+      <c r="Q49" s="6"/>
+      <c r="R49" s="7"/>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A50" s="147" t="s">
         <v>41</v>
       </c>
@@ -3862,10 +4014,10 @@
       <c r="I50" s="149">
         <v>0</v>
       </c>
-      <c r="J50" s="151">
-        <v>0</v>
-      </c>
-      <c r="K50" s="152">
+      <c r="J50" s="154">
+        <v>0</v>
+      </c>
+      <c r="K50" s="151">
         <v>0</v>
       </c>
       <c r="L50" s="152">
@@ -3877,20 +4029,23 @@
       <c r="N50" s="152">
         <v>0</v>
       </c>
-      <c r="O50" s="153">
-        <v>0</v>
-      </c>
-      <c r="P50" s="149">
-        <v>0</v>
-      </c>
-      <c r="Q50" s="154">
-        <v>0</v>
-      </c>
-      <c r="R50" s="204" t="s">
+      <c r="O50" s="152">
+        <v>0</v>
+      </c>
+      <c r="P50" s="153">
+        <v>0</v>
+      </c>
+      <c r="Q50" s="149">
+        <v>0</v>
+      </c>
+      <c r="R50" s="154">
+        <v>0</v>
+      </c>
+      <c r="S50" s="204" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A51" s="155"/>
       <c r="B51" s="156"/>
       <c r="C51" s="170"/>
@@ -3900,14 +4055,15 @@
       <c r="G51" s="6"/>
       <c r="H51" s="133"/>
       <c r="I51" s="6"/>
-      <c r="J51" s="171"/>
-      <c r="K51" s="172"/>
+      <c r="J51" s="7"/>
+      <c r="K51" s="171"/>
       <c r="L51" s="172"/>
       <c r="M51" s="172"/>
       <c r="N51" s="172"/>
-      <c r="O51" s="173"/>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="O51" s="172"/>
+      <c r="P51" s="173"/>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A52" s="159" t="s">
         <v>61</v>
       </c>
@@ -3935,10 +4091,10 @@
       <c r="I52" s="163">
         <v>0</v>
       </c>
-      <c r="J52" s="174">
-        <v>0</v>
-      </c>
-      <c r="K52" s="175">
+      <c r="J52" s="165">
+        <v>0</v>
+      </c>
+      <c r="K52" s="174">
         <v>0</v>
       </c>
       <c r="L52" s="175">
@@ -3950,20 +4106,23 @@
       <c r="N52" s="175">
         <v>0</v>
       </c>
-      <c r="O52" s="178">
-        <v>0</v>
-      </c>
-      <c r="P52" s="163">
-        <v>0</v>
-      </c>
-      <c r="Q52" s="165">
-        <v>0</v>
-      </c>
-      <c r="R52" s="205" t="s">
+      <c r="O52" s="175">
+        <v>0</v>
+      </c>
+      <c r="P52" s="178">
+        <v>0</v>
+      </c>
+      <c r="Q52" s="163">
+        <v>0</v>
+      </c>
+      <c r="R52" s="165">
+        <v>0</v>
+      </c>
+      <c r="S52" s="205" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A53" s="161" t="s">
         <v>62</v>
       </c>
@@ -3991,10 +4150,10 @@
       <c r="I53" s="166">
         <v>0</v>
       </c>
-      <c r="J53" s="176">
-        <v>0</v>
-      </c>
-      <c r="K53" s="177">
+      <c r="J53" s="168">
+        <v>0</v>
+      </c>
+      <c r="K53" s="176">
         <v>0</v>
       </c>
       <c r="L53" s="177">
@@ -4006,20 +4165,23 @@
       <c r="N53" s="177">
         <v>0</v>
       </c>
-      <c r="O53" s="179">
-        <v>0</v>
-      </c>
-      <c r="P53" s="166">
-        <v>0</v>
-      </c>
-      <c r="Q53" s="168">
-        <v>0</v>
-      </c>
-      <c r="R53" s="205" t="s">
+      <c r="O53" s="177">
+        <v>0</v>
+      </c>
+      <c r="P53" s="179">
+        <v>0</v>
+      </c>
+      <c r="Q53" s="166">
+        <v>0</v>
+      </c>
+      <c r="R53" s="168">
+        <v>0</v>
+      </c>
+      <c r="S53" s="205" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A54" s="3"/>
       <c r="B54" s="157"/>
       <c r="C54" s="6"/>
@@ -4029,16 +4191,17 @@
       <c r="G54" s="6"/>
       <c r="H54" s="169"/>
       <c r="I54" s="6"/>
-      <c r="J54" s="17"/>
-      <c r="K54" s="18"/>
+      <c r="J54" s="7"/>
+      <c r="K54" s="17"/>
       <c r="L54" s="18"/>
       <c r="M54" s="18"/>
       <c r="N54" s="18"/>
-      <c r="O54" s="19"/>
-      <c r="P54" s="6"/>
-      <c r="Q54" s="7"/>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="O54" s="18"/>
+      <c r="P54" s="19"/>
+      <c r="Q54" s="6"/>
+      <c r="R54" s="7"/>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A55" s="181" t="s">
         <v>64</v>
       </c>
@@ -4066,10 +4229,10 @@
       <c r="I55" s="184">
         <v>0</v>
       </c>
-      <c r="J55" s="185">
-        <v>0</v>
-      </c>
-      <c r="K55" s="186">
+      <c r="J55" s="221">
+        <v>0</v>
+      </c>
+      <c r="K55" s="185">
         <v>0</v>
       </c>
       <c r="L55" s="186">
@@ -4081,20 +4244,23 @@
       <c r="N55" s="186">
         <v>0</v>
       </c>
-      <c r="O55" s="187">
-        <v>0</v>
-      </c>
-      <c r="P55" s="183">
-        <v>0</v>
-      </c>
-      <c r="Q55" s="188">
-        <v>0</v>
-      </c>
-      <c r="R55" s="202">
+      <c r="O55" s="186">
+        <v>0</v>
+      </c>
+      <c r="P55" s="187">
+        <v>0</v>
+      </c>
+      <c r="Q55" s="183">
+        <v>0</v>
+      </c>
+      <c r="R55" s="188">
+        <v>0</v>
+      </c>
+      <c r="S55" s="202">
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A56" s="189" t="s">
         <v>65</v>
       </c>
@@ -4122,10 +4288,10 @@
       <c r="I56" s="192">
         <v>0</v>
       </c>
-      <c r="J56" s="193">
-        <v>0</v>
-      </c>
-      <c r="K56" s="194">
+      <c r="J56" s="222">
+        <v>0</v>
+      </c>
+      <c r="K56" s="193">
         <v>0</v>
       </c>
       <c r="L56" s="194">
@@ -4137,48 +4303,51 @@
       <c r="N56" s="194">
         <v>0</v>
       </c>
-      <c r="O56" s="195">
-        <v>0</v>
-      </c>
-      <c r="P56" s="191">
-        <v>0</v>
-      </c>
-      <c r="Q56" s="196">
-        <v>0</v>
-      </c>
-      <c r="R56" s="202">
+      <c r="O56" s="194">
+        <v>0</v>
+      </c>
+      <c r="P56" s="195">
+        <v>0</v>
+      </c>
+      <c r="Q56" s="191">
+        <v>0</v>
+      </c>
+      <c r="R56" s="196">
+        <v>0</v>
+      </c>
+      <c r="S56" s="202">
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A57" s="144"/>
       <c r="B57" s="4"/>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
     </row>
@@ -4199,8 +4368,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="J1:O1"/>
-    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="K1:P1"/>
+    <mergeCell ref="T3:U3"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
now load and store is working. test added
</commit_message>
<xml_diff>
--- a/ctrl words dlx.xlsx
+++ b/ctrl words dlx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kelme\Desktop\DLX_git2\DLXproj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FF2F6A-87DF-41E0-98FA-EC3FA221A683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{751E8A1B-25D8-4B73-B534-9CA916501E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{97E78207-76B4-4719-AF3A-2C20865B08CC}"/>
   </bookViews>
@@ -921,12 +921,6 @@
     <xf numFmtId="49" fontId="1" fillId="6" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -941,6 +935,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1272,11 +1272,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FA04DC4-AE17-4075-AF88-F2CFFC720BD3}">
   <dimension ref="A1:U68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W50" sqref="W50"/>
+      <selection pane="bottomRight" activeCell="R47" sqref="R47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1318,14 +1318,14 @@
       <c r="J1" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="K1" s="207" t="s">
+      <c r="K1" s="221" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="207"/>
-      <c r="M1" s="207"/>
-      <c r="N1" s="207"/>
-      <c r="O1" s="207"/>
-      <c r="P1" s="207"/>
+      <c r="L1" s="221"/>
+      <c r="M1" s="221"/>
+      <c r="N1" s="221"/>
+      <c r="O1" s="221"/>
+      <c r="P1" s="221"/>
       <c r="Q1" s="22" t="s">
         <v>29</v>
       </c>
@@ -1364,7 +1364,7 @@
       <c r="I2" s="26">
         <v>0</v>
       </c>
-      <c r="J2" s="209">
+      <c r="J2" s="207">
         <v>1</v>
       </c>
       <c r="K2" s="27">
@@ -1423,7 +1423,7 @@
       <c r="I3" s="26">
         <v>0</v>
       </c>
-      <c r="J3" s="209">
+      <c r="J3" s="207">
         <v>1</v>
       </c>
       <c r="K3" s="27">
@@ -1453,10 +1453,10 @@
       <c r="S3" s="198" t="s">
         <v>69</v>
       </c>
-      <c r="T3" s="208" t="s">
+      <c r="T3" s="222" t="s">
         <v>53</v>
       </c>
-      <c r="U3" s="208"/>
+      <c r="U3" s="222"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
@@ -1486,7 +1486,7 @@
       <c r="I4" s="26">
         <v>0</v>
       </c>
-      <c r="J4" s="209">
+      <c r="J4" s="207">
         <v>1</v>
       </c>
       <c r="K4" s="27">
@@ -1549,7 +1549,7 @@
       <c r="I5" s="26">
         <v>0</v>
       </c>
-      <c r="J5" s="209">
+      <c r="J5" s="207">
         <v>1</v>
       </c>
       <c r="K5" s="27">
@@ -1612,7 +1612,7 @@
       <c r="I6" s="26">
         <v>0</v>
       </c>
-      <c r="J6" s="209">
+      <c r="J6" s="207">
         <v>1</v>
       </c>
       <c r="K6" s="27">
@@ -1675,7 +1675,7 @@
       <c r="I7" s="34">
         <v>0</v>
       </c>
-      <c r="J7" s="210">
+      <c r="J7" s="208">
         <v>1</v>
       </c>
       <c r="K7" s="35">
@@ -1738,7 +1738,7 @@
       <c r="I8" s="26">
         <v>1</v>
       </c>
-      <c r="J8" s="209">
+      <c r="J8" s="207">
         <v>1</v>
       </c>
       <c r="K8" s="27">
@@ -1801,7 +1801,7 @@
       <c r="I9" s="26">
         <v>1</v>
       </c>
-      <c r="J9" s="209">
+      <c r="J9" s="207">
         <v>1</v>
       </c>
       <c r="K9" s="27">
@@ -1864,7 +1864,7 @@
       <c r="I10" s="26">
         <v>1</v>
       </c>
-      <c r="J10" s="209">
+      <c r="J10" s="207">
         <v>1</v>
       </c>
       <c r="K10" s="27">
@@ -1927,7 +1927,7 @@
       <c r="I11" s="26">
         <v>1</v>
       </c>
-      <c r="J11" s="209">
+      <c r="J11" s="207">
         <v>1</v>
       </c>
       <c r="K11" s="27">
@@ -1990,7 +1990,7 @@
       <c r="I12" s="26">
         <v>1</v>
       </c>
-      <c r="J12" s="209">
+      <c r="J12" s="207">
         <v>1</v>
       </c>
       <c r="K12" s="27">
@@ -2053,7 +2053,7 @@
       <c r="I13" s="34">
         <v>1</v>
       </c>
-      <c r="J13" s="210">
+      <c r="J13" s="208">
         <v>1</v>
       </c>
       <c r="K13" s="35">
@@ -2132,7 +2132,7 @@
       <c r="I15" s="44">
         <v>0</v>
       </c>
-      <c r="J15" s="211">
+      <c r="J15" s="209">
         <v>1</v>
       </c>
       <c r="K15" s="45">
@@ -2191,7 +2191,7 @@
       <c r="I16" s="44">
         <v>0</v>
       </c>
-      <c r="J16" s="211">
+      <c r="J16" s="209">
         <v>1</v>
       </c>
       <c r="K16" s="45">
@@ -2250,7 +2250,7 @@
       <c r="I17" s="44">
         <v>1</v>
       </c>
-      <c r="J17" s="211">
+      <c r="J17" s="209">
         <v>1</v>
       </c>
       <c r="K17" s="45">
@@ -2309,7 +2309,7 @@
       <c r="I18" s="53">
         <v>1</v>
       </c>
-      <c r="J18" s="212">
+      <c r="J18" s="210">
         <v>1</v>
       </c>
       <c r="K18" s="54">
@@ -2400,7 +2400,7 @@
       <c r="I20" s="62">
         <v>0</v>
       </c>
-      <c r="J20" s="213">
+      <c r="J20" s="211">
         <v>1</v>
       </c>
       <c r="K20" s="63">
@@ -2459,7 +2459,7 @@
       <c r="I21" s="62">
         <v>0</v>
       </c>
-      <c r="J21" s="213">
+      <c r="J21" s="211">
         <v>1</v>
       </c>
       <c r="K21" s="63">
@@ -2518,7 +2518,7 @@
       <c r="I22" s="62">
         <v>0</v>
       </c>
-      <c r="J22" s="213">
+      <c r="J22" s="211">
         <v>1</v>
       </c>
       <c r="K22" s="63">
@@ -2577,7 +2577,7 @@
       <c r="I23" s="70">
         <v>0</v>
       </c>
-      <c r="J23" s="214">
+      <c r="J23" s="212">
         <v>1</v>
       </c>
       <c r="K23" s="71">
@@ -2636,7 +2636,7 @@
       <c r="I24" s="62">
         <v>1</v>
       </c>
-      <c r="J24" s="213">
+      <c r="J24" s="211">
         <v>1</v>
       </c>
       <c r="K24" s="63">
@@ -2695,7 +2695,7 @@
       <c r="I25" s="62">
         <v>1</v>
       </c>
-      <c r="J25" s="213">
+      <c r="J25" s="211">
         <v>1</v>
       </c>
       <c r="K25" s="63">
@@ -2754,7 +2754,7 @@
       <c r="I26" s="62">
         <v>1</v>
       </c>
-      <c r="J26" s="213">
+      <c r="J26" s="211">
         <v>1</v>
       </c>
       <c r="K26" s="63">
@@ -2813,7 +2813,7 @@
       <c r="I27" s="70">
         <v>1</v>
       </c>
-      <c r="J27" s="214">
+      <c r="J27" s="212">
         <v>1</v>
       </c>
       <c r="K27" s="71">
@@ -2892,7 +2892,7 @@
       <c r="I29" s="79">
         <v>0</v>
       </c>
-      <c r="J29" s="215">
+      <c r="J29" s="213">
         <v>1</v>
       </c>
       <c r="K29" s="80">
@@ -2951,7 +2951,7 @@
       <c r="I30" s="79">
         <v>0</v>
       </c>
-      <c r="J30" s="215">
+      <c r="J30" s="213">
         <v>1</v>
       </c>
       <c r="K30" s="80">
@@ -3010,7 +3010,7 @@
       <c r="I31" s="79">
         <v>0</v>
       </c>
-      <c r="J31" s="215">
+      <c r="J31" s="213">
         <v>1</v>
       </c>
       <c r="K31" s="80">
@@ -3069,7 +3069,7 @@
       <c r="I32" s="79">
         <v>0</v>
       </c>
-      <c r="J32" s="215">
+      <c r="J32" s="213">
         <v>1</v>
       </c>
       <c r="K32" s="80">
@@ -3128,7 +3128,7 @@
       <c r="I33" s="79">
         <v>0</v>
       </c>
-      <c r="J33" s="215">
+      <c r="J33" s="213">
         <v>1</v>
       </c>
       <c r="K33" s="80">
@@ -3187,7 +3187,7 @@
       <c r="I34" s="79">
         <v>0</v>
       </c>
-      <c r="J34" s="215">
+      <c r="J34" s="213">
         <v>1</v>
       </c>
       <c r="K34" s="80">
@@ -3246,7 +3246,7 @@
       <c r="I35" s="87">
         <v>0</v>
       </c>
-      <c r="J35" s="216">
+      <c r="J35" s="214">
         <v>1</v>
       </c>
       <c r="K35" s="88">
@@ -3305,7 +3305,7 @@
       <c r="I36" s="79">
         <v>1</v>
       </c>
-      <c r="J36" s="215">
+      <c r="J36" s="213">
         <v>1</v>
       </c>
       <c r="K36" s="80">
@@ -3364,7 +3364,7 @@
       <c r="I37" s="79">
         <v>1</v>
       </c>
-      <c r="J37" s="215">
+      <c r="J37" s="213">
         <v>1</v>
       </c>
       <c r="K37" s="80">
@@ -3423,7 +3423,7 @@
       <c r="I38" s="79">
         <v>1</v>
       </c>
-      <c r="J38" s="215">
+      <c r="J38" s="213">
         <v>1</v>
       </c>
       <c r="K38" s="80">
@@ -3482,7 +3482,7 @@
       <c r="I39" s="79">
         <v>1</v>
       </c>
-      <c r="J39" s="215">
+      <c r="J39" s="213">
         <v>1</v>
       </c>
       <c r="K39" s="80">
@@ -3541,7 +3541,7 @@
       <c r="I40" s="79">
         <v>1</v>
       </c>
-      <c r="J40" s="215">
+      <c r="J40" s="213">
         <v>1</v>
       </c>
       <c r="K40" s="80">
@@ -3600,7 +3600,7 @@
       <c r="I41" s="79">
         <v>1</v>
       </c>
-      <c r="J41" s="215">
+      <c r="J41" s="213">
         <v>1</v>
       </c>
       <c r="K41" s="80">
@@ -3659,7 +3659,7 @@
       <c r="I42" s="87">
         <v>1</v>
       </c>
-      <c r="J42" s="216">
+      <c r="J42" s="214">
         <v>1</v>
       </c>
       <c r="K42" s="88">
@@ -3738,7 +3738,7 @@
       <c r="I44" s="123">
         <v>0</v>
       </c>
-      <c r="J44" s="217">
+      <c r="J44" s="215">
         <v>1</v>
       </c>
       <c r="K44" s="124">
@@ -3797,7 +3797,7 @@
       <c r="I45" s="96">
         <v>1</v>
       </c>
-      <c r="J45" s="218">
+      <c r="J45" s="216">
         <v>1</v>
       </c>
       <c r="K45" s="97">
@@ -3868,7 +3868,7 @@
         <v>1</v>
       </c>
       <c r="G47" s="106">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H47" s="141">
         <v>0</v>
@@ -3876,7 +3876,7 @@
       <c r="I47" s="106">
         <v>1</v>
       </c>
-      <c r="J47" s="219">
+      <c r="J47" s="217">
         <v>1</v>
       </c>
       <c r="K47" s="107">
@@ -3927,7 +3927,7 @@
         <v>1</v>
       </c>
       <c r="G48" s="114">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H48" s="142">
         <v>0</v>
@@ -3935,7 +3935,7 @@
       <c r="I48" s="114">
         <v>1</v>
       </c>
-      <c r="J48" s="220">
+      <c r="J48" s="218">
         <v>1</v>
       </c>
       <c r="K48" s="115">
@@ -4229,7 +4229,7 @@
       <c r="I55" s="184">
         <v>0</v>
       </c>
-      <c r="J55" s="221">
+      <c r="J55" s="219">
         <v>0</v>
       </c>
       <c r="K55" s="185">
@@ -4288,7 +4288,7 @@
       <c r="I56" s="192">
         <v>0</v>
       </c>
-      <c r="J56" s="222">
+      <c r="J56" s="220">
         <v>0</v>
       </c>
       <c r="K56" s="193">

</xml_diff>

<commit_message>
fixed excel file and CU description
</commit_message>
<xml_diff>
--- a/ctrl words dlx.xlsx
+++ b/ctrl words dlx.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kelme\Desktop\DLX_git2\DLXproj\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kelme\Desktop\DLX_GIT\DLXproj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{751E8A1B-25D8-4B73-B534-9CA916501E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{537F6D54-CFA5-423B-8B0D-BA2DDB2FAADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{97E78207-76B4-4719-AF3A-2C20865B08CC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="70">
   <si>
     <t>BranchD</t>
   </si>
@@ -75,9 +75,6 @@
     <t>SRA</t>
   </si>
   <si>
-    <t>SLA</t>
-  </si>
-  <si>
     <t>SGE</t>
   </si>
   <si>
@@ -139,9 +136,6 @@
   </si>
   <si>
     <t>SEQ</t>
-  </si>
-  <si>
-    <t>SEQZ</t>
   </si>
   <si>
     <t>SNEQ</t>
@@ -1270,13 +1264,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FA04DC4-AE17-4075-AF88-F2CFFC720BD3}">
-  <dimension ref="A1:U68"/>
+  <dimension ref="A1:U66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R47" sqref="R47"/>
+      <selection pane="bottomRight" activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1298,28 +1292,28 @@
         <v>1</v>
       </c>
       <c r="D1" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="F1" s="21" t="s">
+      <c r="G1" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="H1" s="130" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="130" t="s">
+      <c r="I1" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="221" t="s">
         <v>26</v>
-      </c>
-      <c r="I1" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="K1" s="221" t="s">
-        <v>27</v>
       </c>
       <c r="L1" s="221"/>
       <c r="M1" s="221"/>
@@ -1327,13 +1321,13 @@
       <c r="O1" s="221"/>
       <c r="P1" s="221"/>
       <c r="Q1" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R1" s="23" t="s">
         <v>2</v>
       </c>
       <c r="S1" s="197" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -1392,7 +1386,7 @@
         <v>0</v>
       </c>
       <c r="S2" s="198" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
@@ -1451,10 +1445,10 @@
         <v>0</v>
       </c>
       <c r="S3" s="198" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T3" s="222" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="U3" s="222"/>
     </row>
@@ -1514,11 +1508,11 @@
         <v>0</v>
       </c>
       <c r="S4" s="198" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T4" s="41"/>
       <c r="U4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
@@ -1577,11 +1571,11 @@
         <v>0</v>
       </c>
       <c r="S5" s="198" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T5" s="59"/>
       <c r="U5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
@@ -1640,11 +1634,11 @@
         <v>0</v>
       </c>
       <c r="S6" s="198" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T6" s="76"/>
       <c r="U6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
@@ -1703,16 +1697,16 @@
         <v>0</v>
       </c>
       <c r="S7" s="198" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T7" s="93"/>
       <c r="U7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="40">
         <v>0</v>
@@ -1766,16 +1760,16 @@
         <v>0</v>
       </c>
       <c r="S8" s="198" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T8" s="103"/>
       <c r="U8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="40">
         <v>0</v>
@@ -1829,16 +1823,16 @@
         <v>0</v>
       </c>
       <c r="S9" s="198" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T9" s="120"/>
       <c r="U9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="40">
         <v>0</v>
@@ -1892,16 +1886,16 @@
         <v>0</v>
       </c>
       <c r="S10" s="198" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T10" s="146"/>
       <c r="U10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="40">
         <v>0</v>
@@ -1955,16 +1949,16 @@
         <v>0</v>
       </c>
       <c r="S11" s="198" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T11" s="158"/>
       <c r="U11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="40">
         <v>0</v>
@@ -2018,16 +2012,16 @@
         <v>0</v>
       </c>
       <c r="S12" s="198" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T12" s="180"/>
       <c r="U12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="33">
         <v>0</v>
@@ -2081,7 +2075,7 @@
         <v>0</v>
       </c>
       <c r="S13" s="198" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
@@ -2106,7 +2100,7 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="42" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B15" s="43">
         <v>0</v>
@@ -2160,12 +2154,12 @@
         <v>0</v>
       </c>
       <c r="S15" s="199" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="50" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B16" s="43">
         <v>0</v>
@@ -2219,12 +2213,12 @@
         <v>0</v>
       </c>
       <c r="S16" s="199" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="50" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B17" s="43">
         <v>0</v>
@@ -2278,12 +2272,12 @@
         <v>0</v>
       </c>
       <c r="S17" s="199" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="51" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B18" s="52">
         <v>0</v>
@@ -2337,7 +2331,7 @@
         <v>0</v>
       </c>
       <c r="S18" s="199" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
@@ -2428,7 +2422,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="200" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
@@ -2487,7 +2481,7 @@
         <v>0</v>
       </c>
       <c r="S21" s="200" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
@@ -2546,66 +2540,66 @@
         <v>0</v>
       </c>
       <c r="S22" s="200" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A23" s="68" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="69">
-        <v>0</v>
-      </c>
-      <c r="C23" s="70">
-        <v>0</v>
-      </c>
-      <c r="D23" s="70">
-        <v>1</v>
-      </c>
-      <c r="E23" s="70">
-        <v>0</v>
-      </c>
-      <c r="F23" s="70">
-        <v>1</v>
-      </c>
-      <c r="G23" s="70">
-        <v>1</v>
-      </c>
-      <c r="H23" s="137">
-        <v>1</v>
-      </c>
-      <c r="I23" s="70">
-        <v>0</v>
-      </c>
-      <c r="J23" s="212">
-        <v>1</v>
-      </c>
-      <c r="K23" s="71">
-        <v>1</v>
-      </c>
-      <c r="L23" s="72">
-        <v>0</v>
-      </c>
-      <c r="M23" s="72" t="s">
+      <c r="A23" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="61">
+        <v>0</v>
+      </c>
+      <c r="C23" s="62">
+        <v>0</v>
+      </c>
+      <c r="D23" s="62">
+        <v>1</v>
+      </c>
+      <c r="E23" s="62">
+        <v>0</v>
+      </c>
+      <c r="F23" s="62">
+        <v>1</v>
+      </c>
+      <c r="G23" s="62">
+        <v>0</v>
+      </c>
+      <c r="H23" s="136">
+        <v>0</v>
+      </c>
+      <c r="I23" s="62">
+        <v>1</v>
+      </c>
+      <c r="J23" s="211">
+        <v>1</v>
+      </c>
+      <c r="K23" s="63">
+        <v>1</v>
+      </c>
+      <c r="L23" s="64">
+        <v>0</v>
+      </c>
+      <c r="M23" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="N23" s="72">
-        <v>0</v>
-      </c>
-      <c r="O23" s="72">
-        <v>1</v>
-      </c>
-      <c r="P23" s="73">
-        <v>1</v>
-      </c>
-      <c r="Q23" s="74">
-        <v>0</v>
-      </c>
-      <c r="R23" s="75">
+      <c r="N23" s="64">
+        <v>0</v>
+      </c>
+      <c r="O23" s="64">
+        <v>0</v>
+      </c>
+      <c r="P23" s="65">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="66">
+        <v>0</v>
+      </c>
+      <c r="R23" s="67">
         <v>0</v>
       </c>
       <c r="S23" s="200" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
@@ -2655,7 +2649,7 @@
         <v>0</v>
       </c>
       <c r="P24" s="65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q24" s="66">
         <v>0</v>
@@ -2664,7 +2658,7 @@
         <v>0</v>
       </c>
       <c r="S24" s="200" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
@@ -2711,10 +2705,10 @@
         <v>0</v>
       </c>
       <c r="O25" s="64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P25" s="65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q25" s="66">
         <v>0</v>
@@ -2723,150 +2717,150 @@
         <v>0</v>
       </c>
       <c r="S25" s="200" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A26" s="60" t="s">
+      <c r="A26" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="61">
-        <v>0</v>
-      </c>
-      <c r="C26" s="62">
-        <v>0</v>
-      </c>
-      <c r="D26" s="62">
-        <v>1</v>
-      </c>
-      <c r="E26" s="62">
-        <v>0</v>
-      </c>
-      <c r="F26" s="62">
-        <v>1</v>
-      </c>
-      <c r="G26" s="62">
-        <v>0</v>
-      </c>
-      <c r="H26" s="136">
-        <v>0</v>
-      </c>
-      <c r="I26" s="62">
-        <v>1</v>
-      </c>
-      <c r="J26" s="211">
-        <v>1</v>
-      </c>
-      <c r="K26" s="63">
-        <v>1</v>
-      </c>
-      <c r="L26" s="64">
-        <v>0</v>
-      </c>
-      <c r="M26" s="64" t="s">
+      <c r="B26" s="69">
+        <v>0</v>
+      </c>
+      <c r="C26" s="70">
+        <v>0</v>
+      </c>
+      <c r="D26" s="70">
+        <v>1</v>
+      </c>
+      <c r="E26" s="70">
+        <v>0</v>
+      </c>
+      <c r="F26" s="70">
+        <v>1</v>
+      </c>
+      <c r="G26" s="70">
+        <v>0</v>
+      </c>
+      <c r="H26" s="137">
+        <v>0</v>
+      </c>
+      <c r="I26" s="70">
+        <v>1</v>
+      </c>
+      <c r="J26" s="212">
+        <v>1</v>
+      </c>
+      <c r="K26" s="71">
+        <v>1</v>
+      </c>
+      <c r="L26" s="72">
+        <v>0</v>
+      </c>
+      <c r="M26" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="N26" s="64">
-        <v>0</v>
-      </c>
-      <c r="O26" s="64">
-        <v>1</v>
-      </c>
-      <c r="P26" s="65">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="66">
-        <v>0</v>
-      </c>
-      <c r="R26" s="67">
+      <c r="N26" s="72">
+        <v>0</v>
+      </c>
+      <c r="O26" s="72">
+        <v>1</v>
+      </c>
+      <c r="P26" s="73">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="74">
+        <v>0</v>
+      </c>
+      <c r="R26" s="75">
         <v>0</v>
       </c>
       <c r="S26" s="200" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A27" s="68" t="s">
+      <c r="A27" s="2"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="133"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="7"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A28" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="69">
-        <v>0</v>
-      </c>
-      <c r="C27" s="70">
-        <v>0</v>
-      </c>
-      <c r="D27" s="70">
-        <v>1</v>
-      </c>
-      <c r="E27" s="70">
-        <v>0</v>
-      </c>
-      <c r="F27" s="70">
-        <v>1</v>
-      </c>
-      <c r="G27" s="70">
-        <v>0</v>
-      </c>
-      <c r="H27" s="137">
-        <v>0</v>
-      </c>
-      <c r="I27" s="70">
-        <v>1</v>
-      </c>
-      <c r="J27" s="212">
-        <v>1</v>
-      </c>
-      <c r="K27" s="71">
-        <v>1</v>
-      </c>
-      <c r="L27" s="72">
-        <v>0</v>
-      </c>
-      <c r="M27" s="72" t="s">
+      <c r="B28" s="78">
+        <v>0</v>
+      </c>
+      <c r="C28" s="79">
+        <v>0</v>
+      </c>
+      <c r="D28" s="79">
+        <v>1</v>
+      </c>
+      <c r="E28" s="79">
+        <v>0</v>
+      </c>
+      <c r="F28" s="79">
+        <v>1</v>
+      </c>
+      <c r="G28" s="79">
+        <v>1</v>
+      </c>
+      <c r="H28" s="138">
+        <v>1</v>
+      </c>
+      <c r="I28" s="79">
+        <v>0</v>
+      </c>
+      <c r="J28" s="213">
+        <v>1</v>
+      </c>
+      <c r="K28" s="80">
+        <v>1</v>
+      </c>
+      <c r="L28" s="81">
+        <v>1</v>
+      </c>
+      <c r="M28" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="N27" s="72">
-        <v>0</v>
-      </c>
-      <c r="O27" s="72">
-        <v>1</v>
-      </c>
-      <c r="P27" s="73">
-        <v>1</v>
-      </c>
-      <c r="Q27" s="74">
-        <v>0</v>
-      </c>
-      <c r="R27" s="75">
-        <v>0</v>
-      </c>
-      <c r="S27" s="200" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A28" s="2"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="133"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="11"/>
-      <c r="L28" s="12"/>
-      <c r="M28" s="12"/>
-      <c r="N28" s="12"/>
-      <c r="O28" s="12"/>
-      <c r="P28" s="13"/>
-      <c r="Q28" s="6"/>
-      <c r="R28" s="7"/>
+      <c r="N28" s="81">
+        <v>0</v>
+      </c>
+      <c r="O28" s="81">
+        <v>0</v>
+      </c>
+      <c r="P28" s="82">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="83">
+        <v>0</v>
+      </c>
+      <c r="R28" s="84">
+        <v>0</v>
+      </c>
+      <c r="S28" s="201" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="77" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B29" s="78">
         <v>0</v>
@@ -2908,7 +2902,7 @@
         <v>0</v>
       </c>
       <c r="O29" s="81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P29" s="82">
         <v>0</v>
@@ -2920,12 +2914,12 @@
         <v>0</v>
       </c>
       <c r="S29" s="201" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="77" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B30" s="78">
         <v>0</v>
@@ -2967,7 +2961,7 @@
         <v>0</v>
       </c>
       <c r="O30" s="81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P30" s="82">
         <v>1</v>
@@ -2979,12 +2973,12 @@
         <v>0</v>
       </c>
       <c r="S30" s="201" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="77" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31" s="78">
         <v>0</v>
@@ -3023,10 +3017,10 @@
         <v>3</v>
       </c>
       <c r="N31" s="81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O31" s="81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P31" s="82">
         <v>0</v>
@@ -3038,7 +3032,7 @@
         <v>0</v>
       </c>
       <c r="S31" s="201" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
@@ -3082,10 +3076,10 @@
         <v>3</v>
       </c>
       <c r="N32" s="81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O32" s="81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P32" s="82">
         <v>1</v>
@@ -3097,71 +3091,71 @@
         <v>0</v>
       </c>
       <c r="S32" s="201" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A33" s="77" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" s="78">
-        <v>0</v>
-      </c>
-      <c r="C33" s="79">
-        <v>0</v>
-      </c>
-      <c r="D33" s="79">
-        <v>1</v>
-      </c>
-      <c r="E33" s="79">
-        <v>0</v>
-      </c>
-      <c r="F33" s="79">
-        <v>1</v>
-      </c>
-      <c r="G33" s="79">
-        <v>1</v>
-      </c>
-      <c r="H33" s="138">
-        <v>1</v>
-      </c>
-      <c r="I33" s="79">
-        <v>0</v>
-      </c>
-      <c r="J33" s="213">
-        <v>1</v>
-      </c>
-      <c r="K33" s="80">
-        <v>1</v>
-      </c>
-      <c r="L33" s="81">
-        <v>1</v>
-      </c>
-      <c r="M33" s="81" t="s">
+      <c r="A33" s="85" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="86">
+        <v>0</v>
+      </c>
+      <c r="C33" s="87">
+        <v>0</v>
+      </c>
+      <c r="D33" s="87">
+        <v>1</v>
+      </c>
+      <c r="E33" s="87">
+        <v>0</v>
+      </c>
+      <c r="F33" s="87">
+        <v>1</v>
+      </c>
+      <c r="G33" s="87">
+        <v>1</v>
+      </c>
+      <c r="H33" s="145">
+        <v>1</v>
+      </c>
+      <c r="I33" s="87">
+        <v>0</v>
+      </c>
+      <c r="J33" s="214">
+        <v>1</v>
+      </c>
+      <c r="K33" s="88">
+        <v>1</v>
+      </c>
+      <c r="L33" s="89">
+        <v>1</v>
+      </c>
+      <c r="M33" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="N33" s="81">
-        <v>1</v>
-      </c>
-      <c r="O33" s="81">
-        <v>0</v>
-      </c>
-      <c r="P33" s="82">
-        <v>0</v>
-      </c>
-      <c r="Q33" s="83">
-        <v>0</v>
-      </c>
-      <c r="R33" s="84">
+      <c r="N33" s="89">
+        <v>1</v>
+      </c>
+      <c r="O33" s="89">
+        <v>1</v>
+      </c>
+      <c r="P33" s="90">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="91">
+        <v>0</v>
+      </c>
+      <c r="R33" s="92">
         <v>0</v>
       </c>
       <c r="S33" s="201" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" s="77" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B34" s="78">
         <v>0</v>
@@ -3179,13 +3173,13 @@
         <v>1</v>
       </c>
       <c r="G34" s="79">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H34" s="138">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I34" s="79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J34" s="213">
         <v>1</v>
@@ -3200,13 +3194,13 @@
         <v>3</v>
       </c>
       <c r="N34" s="81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O34" s="81">
         <v>0</v>
       </c>
       <c r="P34" s="82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q34" s="83">
         <v>0</v>
@@ -3215,66 +3209,66 @@
         <v>0</v>
       </c>
       <c r="S34" s="201" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A35" s="85" t="s">
-        <v>38</v>
-      </c>
-      <c r="B35" s="86">
-        <v>0</v>
-      </c>
-      <c r="C35" s="87">
-        <v>0</v>
-      </c>
-      <c r="D35" s="87">
-        <v>1</v>
-      </c>
-      <c r="E35" s="87">
-        <v>0</v>
-      </c>
-      <c r="F35" s="87">
-        <v>1</v>
-      </c>
-      <c r="G35" s="87">
-        <v>1</v>
-      </c>
-      <c r="H35" s="145">
-        <v>1</v>
-      </c>
-      <c r="I35" s="87">
-        <v>0</v>
-      </c>
-      <c r="J35" s="214">
-        <v>1</v>
-      </c>
-      <c r="K35" s="88">
-        <v>1</v>
-      </c>
-      <c r="L35" s="89">
-        <v>1</v>
-      </c>
-      <c r="M35" s="89" t="s">
+      <c r="A35" s="77" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" s="78">
+        <v>0</v>
+      </c>
+      <c r="C35" s="79">
+        <v>0</v>
+      </c>
+      <c r="D35" s="79">
+        <v>1</v>
+      </c>
+      <c r="E35" s="79">
+        <v>0</v>
+      </c>
+      <c r="F35" s="79">
+        <v>1</v>
+      </c>
+      <c r="G35" s="79">
+        <v>0</v>
+      </c>
+      <c r="H35" s="138">
+        <v>0</v>
+      </c>
+      <c r="I35" s="79">
+        <v>1</v>
+      </c>
+      <c r="J35" s="213">
+        <v>1</v>
+      </c>
+      <c r="K35" s="80">
+        <v>1</v>
+      </c>
+      <c r="L35" s="81">
+        <v>1</v>
+      </c>
+      <c r="M35" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="N35" s="89">
-        <v>1</v>
-      </c>
-      <c r="O35" s="89">
-        <v>1</v>
-      </c>
-      <c r="P35" s="90">
-        <v>0</v>
-      </c>
-      <c r="Q35" s="91">
-        <v>0</v>
-      </c>
-      <c r="R35" s="92">
+      <c r="N35" s="81">
+        <v>0</v>
+      </c>
+      <c r="O35" s="81">
+        <v>0</v>
+      </c>
+      <c r="P35" s="82">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="83">
+        <v>0</v>
+      </c>
+      <c r="R35" s="84">
         <v>0</v>
       </c>
       <c r="S35" s="201" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.3">
@@ -3321,7 +3315,7 @@
         <v>0</v>
       </c>
       <c r="O36" s="81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P36" s="82">
         <v>0</v>
@@ -3333,7 +3327,7 @@
         <v>0</v>
       </c>
       <c r="S36" s="201" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.3">
@@ -3380,7 +3374,7 @@
         <v>0</v>
       </c>
       <c r="O37" s="81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P37" s="82">
         <v>1</v>
@@ -3392,7 +3386,7 @@
         <v>0</v>
       </c>
       <c r="S37" s="201" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.3">
@@ -3436,10 +3430,10 @@
         <v>3</v>
       </c>
       <c r="N38" s="81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O38" s="81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P38" s="82">
         <v>0</v>
@@ -3451,7 +3445,7 @@
         <v>0</v>
       </c>
       <c r="S38" s="201" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.3">
@@ -3495,10 +3489,10 @@
         <v>3</v>
       </c>
       <c r="N39" s="81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O39" s="81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P39" s="82">
         <v>1</v>
@@ -3510,817 +3504,707 @@
         <v>0</v>
       </c>
       <c r="S39" s="201" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A40" s="77" t="s">
+      <c r="A40" s="85" t="s">
         <v>50</v>
       </c>
-      <c r="B40" s="78">
-        <v>0</v>
-      </c>
-      <c r="C40" s="79">
-        <v>0</v>
-      </c>
-      <c r="D40" s="79">
-        <v>1</v>
-      </c>
-      <c r="E40" s="79">
-        <v>0</v>
-      </c>
-      <c r="F40" s="79">
-        <v>1</v>
-      </c>
-      <c r="G40" s="79">
+      <c r="B40" s="86">
+        <v>0</v>
+      </c>
+      <c r="C40" s="87">
+        <v>0</v>
+      </c>
+      <c r="D40" s="87">
+        <v>1</v>
+      </c>
+      <c r="E40" s="87">
+        <v>0</v>
+      </c>
+      <c r="F40" s="87">
+        <v>1</v>
+      </c>
+      <c r="G40" s="87">
         <v>0</v>
       </c>
       <c r="H40" s="138">
         <v>0</v>
       </c>
-      <c r="I40" s="79">
-        <v>1</v>
-      </c>
-      <c r="J40" s="213">
-        <v>1</v>
-      </c>
-      <c r="K40" s="80">
-        <v>1</v>
-      </c>
-      <c r="L40" s="81">
-        <v>1</v>
-      </c>
-      <c r="M40" s="81" t="s">
+      <c r="I40" s="87">
+        <v>1</v>
+      </c>
+      <c r="J40" s="214">
+        <v>1</v>
+      </c>
+      <c r="K40" s="88">
+        <v>1</v>
+      </c>
+      <c r="L40" s="89">
+        <v>1</v>
+      </c>
+      <c r="M40" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="N40" s="81">
-        <v>1</v>
-      </c>
-      <c r="O40" s="81">
-        <v>0</v>
-      </c>
-      <c r="P40" s="82">
-        <v>0</v>
-      </c>
-      <c r="Q40" s="83">
-        <v>0</v>
-      </c>
-      <c r="R40" s="84">
+      <c r="N40" s="89">
+        <v>1</v>
+      </c>
+      <c r="O40" s="89">
+        <v>1</v>
+      </c>
+      <c r="P40" s="90">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="91">
+        <v>0</v>
+      </c>
+      <c r="R40" s="92">
         <v>0</v>
       </c>
       <c r="S40" s="201" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A41" s="77" t="s">
-        <v>51</v>
-      </c>
-      <c r="B41" s="78">
-        <v>0</v>
-      </c>
-      <c r="C41" s="79">
-        <v>0</v>
-      </c>
-      <c r="D41" s="79">
-        <v>1</v>
-      </c>
-      <c r="E41" s="79">
-        <v>0</v>
-      </c>
-      <c r="F41" s="79">
-        <v>1</v>
-      </c>
-      <c r="G41" s="79">
-        <v>0</v>
-      </c>
-      <c r="H41" s="138">
-        <v>0</v>
-      </c>
-      <c r="I41" s="79">
-        <v>1</v>
-      </c>
-      <c r="J41" s="213">
-        <v>1</v>
-      </c>
-      <c r="K41" s="80">
-        <v>1</v>
-      </c>
-      <c r="L41" s="81">
-        <v>1</v>
-      </c>
-      <c r="M41" s="81" t="s">
+      <c r="A41" s="1"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="133"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="11"/>
+      <c r="L41" s="12"/>
+      <c r="M41" s="12"/>
+      <c r="N41" s="12"/>
+      <c r="O41" s="12"/>
+      <c r="P41" s="13"/>
+      <c r="Q41" s="8"/>
+      <c r="R41" s="9"/>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A42" s="121" t="s">
+        <v>15</v>
+      </c>
+      <c r="B42" s="122">
+        <v>0</v>
+      </c>
+      <c r="C42" s="123">
+        <v>0</v>
+      </c>
+      <c r="D42" s="123">
+        <v>1</v>
+      </c>
+      <c r="E42" s="123">
+        <v>0</v>
+      </c>
+      <c r="F42" s="123">
+        <v>1</v>
+      </c>
+      <c r="G42" s="123">
+        <v>1</v>
+      </c>
+      <c r="H42" s="139">
+        <v>1</v>
+      </c>
+      <c r="I42" s="123">
+        <v>0</v>
+      </c>
+      <c r="J42" s="215">
+        <v>1</v>
+      </c>
+      <c r="K42" s="124">
+        <v>1</v>
+      </c>
+      <c r="L42" s="125">
+        <v>1</v>
+      </c>
+      <c r="M42" s="126">
+        <v>1</v>
+      </c>
+      <c r="N42" s="125">
+        <v>1</v>
+      </c>
+      <c r="O42" s="125">
+        <v>1</v>
+      </c>
+      <c r="P42" s="127">
+        <v>1</v>
+      </c>
+      <c r="Q42" s="128">
+        <v>0</v>
+      </c>
+      <c r="R42" s="129">
+        <v>0</v>
+      </c>
+      <c r="S42" s="206" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A43" s="94" t="s">
+        <v>58</v>
+      </c>
+      <c r="B43" s="95">
+        <v>0</v>
+      </c>
+      <c r="C43" s="96">
+        <v>0</v>
+      </c>
+      <c r="D43" s="96">
+        <v>1</v>
+      </c>
+      <c r="E43" s="96">
+        <v>0</v>
+      </c>
+      <c r="F43" s="96">
+        <v>1</v>
+      </c>
+      <c r="G43" s="96">
+        <v>0</v>
+      </c>
+      <c r="H43" s="140">
+        <v>0</v>
+      </c>
+      <c r="I43" s="96">
+        <v>1</v>
+      </c>
+      <c r="J43" s="216">
+        <v>1</v>
+      </c>
+      <c r="K43" s="97">
+        <v>1</v>
+      </c>
+      <c r="L43" s="98">
+        <v>1</v>
+      </c>
+      <c r="M43" s="99">
+        <v>1</v>
+      </c>
+      <c r="N43" s="98">
+        <v>1</v>
+      </c>
+      <c r="O43" s="98">
+        <v>1</v>
+      </c>
+      <c r="P43" s="100">
+        <v>1</v>
+      </c>
+      <c r="Q43" s="101">
+        <v>0</v>
+      </c>
+      <c r="R43" s="102">
+        <v>0</v>
+      </c>
+      <c r="S43" s="206" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A44" s="3"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="133"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="14"/>
+      <c r="L44" s="15"/>
+      <c r="M44" s="15"/>
+      <c r="N44" s="15"/>
+      <c r="O44" s="15"/>
+      <c r="P44" s="16"/>
+      <c r="Q44" s="6"/>
+      <c r="R44" s="7"/>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A45" s="104" t="s">
+        <v>37</v>
+      </c>
+      <c r="B45" s="105">
+        <v>0</v>
+      </c>
+      <c r="C45" s="106">
+        <v>0</v>
+      </c>
+      <c r="D45" s="106">
+        <v>1</v>
+      </c>
+      <c r="E45" s="106">
+        <v>0</v>
+      </c>
+      <c r="F45" s="106">
+        <v>1</v>
+      </c>
+      <c r="G45" s="106">
+        <v>1</v>
+      </c>
+      <c r="H45" s="141">
+        <v>0</v>
+      </c>
+      <c r="I45" s="106">
+        <v>1</v>
+      </c>
+      <c r="J45" s="217">
+        <v>1</v>
+      </c>
+      <c r="K45" s="107">
+        <v>0</v>
+      </c>
+      <c r="L45" s="108">
+        <v>1</v>
+      </c>
+      <c r="M45" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="N41" s="81">
-        <v>1</v>
-      </c>
-      <c r="O41" s="81">
-        <v>0</v>
-      </c>
-      <c r="P41" s="82">
-        <v>1</v>
-      </c>
-      <c r="Q41" s="83">
-        <v>0</v>
-      </c>
-      <c r="R41" s="84">
-        <v>0</v>
-      </c>
-      <c r="S41" s="201" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A42" s="85" t="s">
-        <v>52</v>
-      </c>
-      <c r="B42" s="86">
-        <v>0</v>
-      </c>
-      <c r="C42" s="87">
-        <v>0</v>
-      </c>
-      <c r="D42" s="87">
-        <v>1</v>
-      </c>
-      <c r="E42" s="87">
-        <v>0</v>
-      </c>
-      <c r="F42" s="87">
-        <v>1</v>
-      </c>
-      <c r="G42" s="87">
-        <v>0</v>
-      </c>
-      <c r="H42" s="138">
-        <v>0</v>
-      </c>
-      <c r="I42" s="87">
-        <v>1</v>
-      </c>
-      <c r="J42" s="214">
-        <v>1</v>
-      </c>
-      <c r="K42" s="88">
-        <v>1</v>
-      </c>
-      <c r="L42" s="89">
-        <v>1</v>
-      </c>
-      <c r="M42" s="89" t="s">
+      <c r="N45" s="108">
+        <v>0</v>
+      </c>
+      <c r="O45" s="108">
+        <v>0</v>
+      </c>
+      <c r="P45" s="109">
+        <v>0</v>
+      </c>
+      <c r="Q45" s="110">
+        <v>0</v>
+      </c>
+      <c r="R45" s="111">
+        <v>1</v>
+      </c>
+      <c r="S45" s="203" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A46" s="112" t="s">
+        <v>38</v>
+      </c>
+      <c r="B46" s="113">
+        <v>0</v>
+      </c>
+      <c r="C46" s="114">
+        <v>0</v>
+      </c>
+      <c r="D46" s="114">
+        <v>0</v>
+      </c>
+      <c r="E46" s="114">
+        <v>0</v>
+      </c>
+      <c r="F46" s="114">
+        <v>1</v>
+      </c>
+      <c r="G46" s="114">
+        <v>1</v>
+      </c>
+      <c r="H46" s="142">
+        <v>0</v>
+      </c>
+      <c r="I46" s="114">
+        <v>1</v>
+      </c>
+      <c r="J46" s="218">
+        <v>1</v>
+      </c>
+      <c r="K46" s="115">
+        <v>0</v>
+      </c>
+      <c r="L46" s="116">
+        <v>1</v>
+      </c>
+      <c r="M46" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="N42" s="89">
-        <v>1</v>
-      </c>
-      <c r="O42" s="89">
-        <v>1</v>
-      </c>
-      <c r="P42" s="90">
-        <v>0</v>
-      </c>
-      <c r="Q42" s="91">
-        <v>0</v>
-      </c>
-      <c r="R42" s="92">
-        <v>0</v>
-      </c>
-      <c r="S42" s="201" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A43" s="1"/>
-      <c r="B43" s="10"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="133"/>
-      <c r="I43" s="6"/>
-      <c r="J43" s="7"/>
-      <c r="K43" s="11"/>
-      <c r="L43" s="12"/>
-      <c r="M43" s="12"/>
-      <c r="N43" s="12"/>
-      <c r="O43" s="12"/>
-      <c r="P43" s="13"/>
-      <c r="Q43" s="8"/>
-      <c r="R43" s="9"/>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A44" s="121" t="s">
-        <v>16</v>
-      </c>
-      <c r="B44" s="122">
-        <v>0</v>
-      </c>
-      <c r="C44" s="123">
-        <v>0</v>
-      </c>
-      <c r="D44" s="123">
-        <v>1</v>
-      </c>
-      <c r="E44" s="123">
-        <v>0</v>
-      </c>
-      <c r="F44" s="123">
-        <v>1</v>
-      </c>
-      <c r="G44" s="123">
-        <v>1</v>
-      </c>
-      <c r="H44" s="139">
-        <v>1</v>
-      </c>
-      <c r="I44" s="123">
-        <v>0</v>
-      </c>
-      <c r="J44" s="215">
-        <v>1</v>
-      </c>
-      <c r="K44" s="124">
-        <v>1</v>
-      </c>
-      <c r="L44" s="125">
-        <v>1</v>
-      </c>
-      <c r="M44" s="126">
-        <v>1</v>
-      </c>
-      <c r="N44" s="125">
-        <v>1</v>
-      </c>
-      <c r="O44" s="125">
-        <v>1</v>
-      </c>
-      <c r="P44" s="127">
-        <v>1</v>
-      </c>
-      <c r="Q44" s="128">
-        <v>0</v>
-      </c>
-      <c r="R44" s="129">
-        <v>0</v>
-      </c>
-      <c r="S44" s="206" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A45" s="94" t="s">
-        <v>60</v>
-      </c>
-      <c r="B45" s="95">
-        <v>0</v>
-      </c>
-      <c r="C45" s="96">
-        <v>0</v>
-      </c>
-      <c r="D45" s="96">
-        <v>1</v>
-      </c>
-      <c r="E45" s="96">
-        <v>0</v>
-      </c>
-      <c r="F45" s="96">
-        <v>1</v>
-      </c>
-      <c r="G45" s="96">
-        <v>0</v>
-      </c>
-      <c r="H45" s="140">
-        <v>0</v>
-      </c>
-      <c r="I45" s="96">
-        <v>1</v>
-      </c>
-      <c r="J45" s="216">
-        <v>1</v>
-      </c>
-      <c r="K45" s="97">
-        <v>1</v>
-      </c>
-      <c r="L45" s="98">
-        <v>1</v>
-      </c>
-      <c r="M45" s="99">
-        <v>1</v>
-      </c>
-      <c r="N45" s="98">
-        <v>1</v>
-      </c>
-      <c r="O45" s="98">
-        <v>1</v>
-      </c>
-      <c r="P45" s="100">
-        <v>1</v>
-      </c>
-      <c r="Q45" s="101">
-        <v>0</v>
-      </c>
-      <c r="R45" s="102">
-        <v>0</v>
-      </c>
-      <c r="S45" s="206" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A46" s="3"/>
-      <c r="B46" s="10"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="133"/>
-      <c r="I46" s="6"/>
-      <c r="J46" s="7"/>
-      <c r="K46" s="14"/>
-      <c r="L46" s="15"/>
-      <c r="M46" s="15"/>
-      <c r="N46" s="15"/>
-      <c r="O46" s="15"/>
-      <c r="P46" s="16"/>
-      <c r="Q46" s="6"/>
-      <c r="R46" s="7"/>
+      <c r="N46" s="116">
+        <v>0</v>
+      </c>
+      <c r="O46" s="116">
+        <v>0</v>
+      </c>
+      <c r="P46" s="117">
+        <v>0</v>
+      </c>
+      <c r="Q46" s="118">
+        <v>1</v>
+      </c>
+      <c r="R46" s="119">
+        <v>0</v>
+      </c>
+      <c r="S46" s="203" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A47" s="104" t="s">
+      <c r="A47" s="3"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="133"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="17"/>
+      <c r="L47" s="18"/>
+      <c r="M47" s="18"/>
+      <c r="N47" s="18"/>
+      <c r="O47" s="18"/>
+      <c r="P47" s="19"/>
+      <c r="Q47" s="6"/>
+      <c r="R47" s="7"/>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A48" s="147" t="s">
         <v>39</v>
       </c>
-      <c r="B47" s="105">
-        <v>0</v>
-      </c>
-      <c r="C47" s="106">
-        <v>0</v>
-      </c>
-      <c r="D47" s="106">
-        <v>1</v>
-      </c>
-      <c r="E47" s="106">
-        <v>0</v>
-      </c>
-      <c r="F47" s="106">
-        <v>1</v>
-      </c>
-      <c r="G47" s="106">
-        <v>1</v>
-      </c>
-      <c r="H47" s="141">
-        <v>0</v>
-      </c>
-      <c r="I47" s="106">
-        <v>1</v>
-      </c>
-      <c r="J47" s="217">
-        <v>1</v>
-      </c>
-      <c r="K47" s="107">
-        <v>0</v>
-      </c>
-      <c r="L47" s="108">
-        <v>1</v>
-      </c>
-      <c r="M47" s="108" t="s">
-        <v>3</v>
-      </c>
-      <c r="N47" s="108">
-        <v>0</v>
-      </c>
-      <c r="O47" s="108">
-        <v>0</v>
-      </c>
-      <c r="P47" s="109">
-        <v>0</v>
-      </c>
-      <c r="Q47" s="110">
-        <v>0</v>
-      </c>
-      <c r="R47" s="111">
-        <v>1</v>
-      </c>
-      <c r="S47" s="203" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A48" s="112" t="s">
-        <v>40</v>
-      </c>
-      <c r="B48" s="113">
-        <v>0</v>
-      </c>
-      <c r="C48" s="114">
-        <v>0</v>
-      </c>
-      <c r="D48" s="114">
-        <v>0</v>
-      </c>
-      <c r="E48" s="114">
-        <v>0</v>
-      </c>
-      <c r="F48" s="114">
-        <v>1</v>
-      </c>
-      <c r="G48" s="114">
-        <v>1</v>
-      </c>
-      <c r="H48" s="142">
-        <v>0</v>
-      </c>
-      <c r="I48" s="114">
-        <v>1</v>
-      </c>
-      <c r="J48" s="218">
-        <v>1</v>
-      </c>
-      <c r="K48" s="115">
-        <v>0</v>
-      </c>
-      <c r="L48" s="116">
-        <v>1</v>
-      </c>
-      <c r="M48" s="116" t="s">
-        <v>3</v>
-      </c>
-      <c r="N48" s="116">
-        <v>0</v>
-      </c>
-      <c r="O48" s="116">
-        <v>0</v>
-      </c>
-      <c r="P48" s="117">
-        <v>0</v>
-      </c>
-      <c r="Q48" s="118">
-        <v>1</v>
-      </c>
-      <c r="R48" s="119">
-        <v>0</v>
-      </c>
-      <c r="S48" s="203" t="s">
-        <v>69</v>
+      <c r="B48" s="148">
+        <v>0</v>
+      </c>
+      <c r="C48" s="149">
+        <v>0</v>
+      </c>
+      <c r="D48" s="149">
+        <v>0</v>
+      </c>
+      <c r="E48" s="149">
+        <v>0</v>
+      </c>
+      <c r="F48" s="149">
+        <v>0</v>
+      </c>
+      <c r="G48" s="149">
+        <v>0</v>
+      </c>
+      <c r="H48" s="150">
+        <v>0</v>
+      </c>
+      <c r="I48" s="149">
+        <v>0</v>
+      </c>
+      <c r="J48" s="154">
+        <v>0</v>
+      </c>
+      <c r="K48" s="151">
+        <v>0</v>
+      </c>
+      <c r="L48" s="152">
+        <v>0</v>
+      </c>
+      <c r="M48" s="152">
+        <v>0</v>
+      </c>
+      <c r="N48" s="152">
+        <v>0</v>
+      </c>
+      <c r="O48" s="152">
+        <v>0</v>
+      </c>
+      <c r="P48" s="153">
+        <v>0</v>
+      </c>
+      <c r="Q48" s="149">
+        <v>0</v>
+      </c>
+      <c r="R48" s="154">
+        <v>0</v>
+      </c>
+      <c r="S48" s="204" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A49" s="3"/>
-      <c r="B49" s="10"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
+      <c r="A49" s="155"/>
+      <c r="B49" s="156"/>
+      <c r="C49" s="170"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
       <c r="G49" s="6"/>
       <c r="H49" s="133"/>
       <c r="I49" s="6"/>
       <c r="J49" s="7"/>
-      <c r="K49" s="17"/>
-      <c r="L49" s="18"/>
-      <c r="M49" s="18"/>
-      <c r="N49" s="18"/>
-      <c r="O49" s="18"/>
-      <c r="P49" s="19"/>
-      <c r="Q49" s="6"/>
-      <c r="R49" s="7"/>
+      <c r="K49" s="171"/>
+      <c r="L49" s="172"/>
+      <c r="M49" s="172"/>
+      <c r="N49" s="172"/>
+      <c r="O49" s="172"/>
+      <c r="P49" s="173"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A50" s="147" t="s">
-        <v>41</v>
-      </c>
-      <c r="B50" s="148">
-        <v>0</v>
-      </c>
-      <c r="C50" s="149">
-        <v>0</v>
-      </c>
-      <c r="D50" s="149">
-        <v>0</v>
-      </c>
-      <c r="E50" s="149">
-        <v>0</v>
-      </c>
-      <c r="F50" s="149">
-        <v>0</v>
-      </c>
-      <c r="G50" s="149">
-        <v>0</v>
-      </c>
-      <c r="H50" s="150">
-        <v>0</v>
-      </c>
-      <c r="I50" s="149">
-        <v>0</v>
-      </c>
-      <c r="J50" s="154">
-        <v>0</v>
-      </c>
-      <c r="K50" s="151">
-        <v>0</v>
-      </c>
-      <c r="L50" s="152">
-        <v>0</v>
-      </c>
-      <c r="M50" s="152">
-        <v>0</v>
-      </c>
-      <c r="N50" s="152">
-        <v>0</v>
-      </c>
-      <c r="O50" s="152">
-        <v>0</v>
-      </c>
-      <c r="P50" s="153">
-        <v>0</v>
-      </c>
-      <c r="Q50" s="149">
-        <v>0</v>
-      </c>
-      <c r="R50" s="154">
-        <v>0</v>
-      </c>
-      <c r="S50" s="204" t="s">
-        <v>69</v>
+      <c r="A50" s="159" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50" s="160">
+        <v>1</v>
+      </c>
+      <c r="C50" s="163">
+        <v>1</v>
+      </c>
+      <c r="D50" s="163">
+        <v>0</v>
+      </c>
+      <c r="E50" s="163">
+        <v>0</v>
+      </c>
+      <c r="F50" s="163">
+        <v>0</v>
+      </c>
+      <c r="G50" s="163">
+        <v>0</v>
+      </c>
+      <c r="H50" s="164">
+        <v>0</v>
+      </c>
+      <c r="I50" s="163">
+        <v>0</v>
+      </c>
+      <c r="J50" s="165">
+        <v>0</v>
+      </c>
+      <c r="K50" s="174">
+        <v>0</v>
+      </c>
+      <c r="L50" s="175">
+        <v>0</v>
+      </c>
+      <c r="M50" s="175">
+        <v>0</v>
+      </c>
+      <c r="N50" s="175">
+        <v>0</v>
+      </c>
+      <c r="O50" s="175">
+        <v>0</v>
+      </c>
+      <c r="P50" s="178">
+        <v>0</v>
+      </c>
+      <c r="Q50" s="163">
+        <v>0</v>
+      </c>
+      <c r="R50" s="165">
+        <v>0</v>
+      </c>
+      <c r="S50" s="205" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A51" s="155"/>
-      <c r="B51" s="156"/>
-      <c r="C51" s="170"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
-      <c r="H51" s="133"/>
-      <c r="I51" s="6"/>
-      <c r="J51" s="7"/>
-      <c r="K51" s="171"/>
-      <c r="L51" s="172"/>
-      <c r="M51" s="172"/>
-      <c r="N51" s="172"/>
-      <c r="O51" s="172"/>
-      <c r="P51" s="173"/>
+      <c r="A51" s="161" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51" s="162">
+        <v>1</v>
+      </c>
+      <c r="C51" s="166">
+        <v>1</v>
+      </c>
+      <c r="D51" s="166">
+        <v>1</v>
+      </c>
+      <c r="E51" s="166">
+        <v>1</v>
+      </c>
+      <c r="F51" s="166">
+        <v>0</v>
+      </c>
+      <c r="G51" s="166">
+        <v>0</v>
+      </c>
+      <c r="H51" s="167">
+        <v>0</v>
+      </c>
+      <c r="I51" s="166">
+        <v>0</v>
+      </c>
+      <c r="J51" s="168">
+        <v>0</v>
+      </c>
+      <c r="K51" s="176">
+        <v>0</v>
+      </c>
+      <c r="L51" s="177">
+        <v>0</v>
+      </c>
+      <c r="M51" s="177">
+        <v>0</v>
+      </c>
+      <c r="N51" s="177">
+        <v>0</v>
+      </c>
+      <c r="O51" s="177">
+        <v>0</v>
+      </c>
+      <c r="P51" s="179">
+        <v>0</v>
+      </c>
+      <c r="Q51" s="166">
+        <v>0</v>
+      </c>
+      <c r="R51" s="168">
+        <v>0</v>
+      </c>
+      <c r="S51" s="205" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A52" s="159" t="s">
-        <v>61</v>
-      </c>
-      <c r="B52" s="160">
-        <v>1</v>
-      </c>
-      <c r="C52" s="163">
-        <v>1</v>
-      </c>
-      <c r="D52" s="163">
-        <v>0</v>
-      </c>
-      <c r="E52" s="163">
-        <v>0</v>
-      </c>
-      <c r="F52" s="163">
-        <v>0</v>
-      </c>
-      <c r="G52" s="163">
-        <v>0</v>
-      </c>
-      <c r="H52" s="164">
-        <v>0</v>
-      </c>
-      <c r="I52" s="163">
-        <v>0</v>
-      </c>
-      <c r="J52" s="165">
-        <v>0</v>
-      </c>
-      <c r="K52" s="174">
-        <v>0</v>
-      </c>
-      <c r="L52" s="175">
-        <v>0</v>
-      </c>
-      <c r="M52" s="175">
-        <v>0</v>
-      </c>
-      <c r="N52" s="175">
-        <v>0</v>
-      </c>
-      <c r="O52" s="175">
-        <v>0</v>
-      </c>
-      <c r="P52" s="178">
-        <v>0</v>
-      </c>
-      <c r="Q52" s="163">
-        <v>0</v>
-      </c>
-      <c r="R52" s="165">
-        <v>0</v>
-      </c>
-      <c r="S52" s="205" t="s">
-        <v>70</v>
-      </c>
+      <c r="A52" s="3"/>
+      <c r="B52" s="157"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="169"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="7"/>
+      <c r="K52" s="17"/>
+      <c r="L52" s="18"/>
+      <c r="M52" s="18"/>
+      <c r="N52" s="18"/>
+      <c r="O52" s="18"/>
+      <c r="P52" s="19"/>
+      <c r="Q52" s="6"/>
+      <c r="R52" s="7"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A53" s="161" t="s">
+      <c r="A53" s="181" t="s">
         <v>62</v>
       </c>
-      <c r="B53" s="162">
-        <v>1</v>
-      </c>
-      <c r="C53" s="166">
-        <v>1</v>
-      </c>
-      <c r="D53" s="166">
-        <v>1</v>
-      </c>
-      <c r="E53" s="166">
-        <v>1</v>
-      </c>
-      <c r="F53" s="166">
-        <v>0</v>
-      </c>
-      <c r="G53" s="166">
-        <v>0</v>
-      </c>
-      <c r="H53" s="167">
-        <v>0</v>
-      </c>
-      <c r="I53" s="166">
-        <v>0</v>
-      </c>
-      <c r="J53" s="168">
-        <v>0</v>
-      </c>
-      <c r="K53" s="176">
-        <v>0</v>
-      </c>
-      <c r="L53" s="177">
-        <v>0</v>
-      </c>
-      <c r="M53" s="177">
-        <v>0</v>
-      </c>
-      <c r="N53" s="177">
-        <v>0</v>
-      </c>
-      <c r="O53" s="177">
-        <v>0</v>
-      </c>
-      <c r="P53" s="179">
-        <v>0</v>
-      </c>
-      <c r="Q53" s="166">
-        <v>0</v>
-      </c>
-      <c r="R53" s="168">
-        <v>0</v>
-      </c>
-      <c r="S53" s="205" t="s">
-        <v>70</v>
+      <c r="B53" s="182">
+        <v>1</v>
+      </c>
+      <c r="C53" s="183">
+        <v>0</v>
+      </c>
+      <c r="D53" s="183">
+        <v>0</v>
+      </c>
+      <c r="E53" s="183">
+        <v>0</v>
+      </c>
+      <c r="F53" s="183">
+        <v>1</v>
+      </c>
+      <c r="G53" s="183">
+        <v>1</v>
+      </c>
+      <c r="H53" s="184">
+        <v>0</v>
+      </c>
+      <c r="I53" s="184">
+        <v>0</v>
+      </c>
+      <c r="J53" s="219">
+        <v>0</v>
+      </c>
+      <c r="K53" s="185">
+        <v>0</v>
+      </c>
+      <c r="L53" s="186">
+        <v>0</v>
+      </c>
+      <c r="M53" s="186">
+        <v>0</v>
+      </c>
+      <c r="N53" s="186">
+        <v>0</v>
+      </c>
+      <c r="O53" s="186">
+        <v>0</v>
+      </c>
+      <c r="P53" s="187">
+        <v>0</v>
+      </c>
+      <c r="Q53" s="183">
+        <v>0</v>
+      </c>
+      <c r="R53" s="188">
+        <v>0</v>
+      </c>
+      <c r="S53" s="202">
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A54" s="3"/>
-      <c r="B54" s="157"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="6"/>
-      <c r="G54" s="6"/>
-      <c r="H54" s="169"/>
-      <c r="I54" s="6"/>
-      <c r="J54" s="7"/>
-      <c r="K54" s="17"/>
-      <c r="L54" s="18"/>
-      <c r="M54" s="18"/>
-      <c r="N54" s="18"/>
-      <c r="O54" s="18"/>
-      <c r="P54" s="19"/>
-      <c r="Q54" s="6"/>
-      <c r="R54" s="7"/>
+      <c r="A54" s="189" t="s">
+        <v>63</v>
+      </c>
+      <c r="B54" s="190">
+        <v>1</v>
+      </c>
+      <c r="C54" s="191">
+        <v>0</v>
+      </c>
+      <c r="D54" s="191">
+        <v>0</v>
+      </c>
+      <c r="E54" s="191">
+        <v>0</v>
+      </c>
+      <c r="F54" s="191">
+        <v>1</v>
+      </c>
+      <c r="G54" s="191">
+        <v>1</v>
+      </c>
+      <c r="H54" s="192">
+        <v>0</v>
+      </c>
+      <c r="I54" s="192">
+        <v>0</v>
+      </c>
+      <c r="J54" s="220">
+        <v>0</v>
+      </c>
+      <c r="K54" s="193">
+        <v>0</v>
+      </c>
+      <c r="L54" s="194">
+        <v>0</v>
+      </c>
+      <c r="M54" s="194">
+        <v>0</v>
+      </c>
+      <c r="N54" s="194">
+        <v>0</v>
+      </c>
+      <c r="O54" s="194">
+        <v>0</v>
+      </c>
+      <c r="P54" s="195">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="191">
+        <v>0</v>
+      </c>
+      <c r="R54" s="196">
+        <v>0</v>
+      </c>
+      <c r="S54" s="202">
+        <v>11</v>
+      </c>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A55" s="181" t="s">
-        <v>64</v>
-      </c>
-      <c r="B55" s="182">
-        <v>1</v>
-      </c>
-      <c r="C55" s="183">
-        <v>0</v>
-      </c>
-      <c r="D55" s="183">
-        <v>0</v>
-      </c>
-      <c r="E55" s="183">
-        <v>0</v>
-      </c>
-      <c r="F55" s="183">
-        <v>1</v>
-      </c>
-      <c r="G55" s="183">
-        <v>1</v>
-      </c>
-      <c r="H55" s="184">
-        <v>0</v>
-      </c>
-      <c r="I55" s="184">
-        <v>0</v>
-      </c>
-      <c r="J55" s="219">
-        <v>0</v>
-      </c>
-      <c r="K55" s="185">
-        <v>0</v>
-      </c>
-      <c r="L55" s="186">
-        <v>0</v>
-      </c>
-      <c r="M55" s="186">
-        <v>0</v>
-      </c>
-      <c r="N55" s="186">
-        <v>0</v>
-      </c>
-      <c r="O55" s="186">
-        <v>0</v>
-      </c>
-      <c r="P55" s="187">
-        <v>0</v>
-      </c>
-      <c r="Q55" s="183">
-        <v>0</v>
-      </c>
-      <c r="R55" s="188">
-        <v>0</v>
-      </c>
-      <c r="S55" s="202">
-        <v>10</v>
-      </c>
+      <c r="A55" s="144"/>
+      <c r="B55" s="4"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A56" s="189" t="s">
-        <v>65</v>
-      </c>
-      <c r="B56" s="190">
-        <v>1</v>
-      </c>
-      <c r="C56" s="191">
-        <v>0</v>
-      </c>
-      <c r="D56" s="191">
-        <v>0</v>
-      </c>
-      <c r="E56" s="191">
-        <v>0</v>
-      </c>
-      <c r="F56" s="191">
-        <v>1</v>
-      </c>
-      <c r="G56" s="191">
-        <v>1</v>
-      </c>
-      <c r="H56" s="192">
-        <v>0</v>
-      </c>
-      <c r="I56" s="192">
-        <v>0</v>
-      </c>
-      <c r="J56" s="220">
-        <v>0</v>
-      </c>
-      <c r="K56" s="193">
-        <v>0</v>
-      </c>
-      <c r="L56" s="194">
-        <v>0</v>
-      </c>
-      <c r="M56" s="194">
-        <v>0</v>
-      </c>
-      <c r="N56" s="194">
-        <v>0</v>
-      </c>
-      <c r="O56" s="194">
-        <v>0</v>
-      </c>
-      <c r="P56" s="195">
-        <v>0</v>
-      </c>
-      <c r="Q56" s="191">
-        <v>0</v>
-      </c>
-      <c r="R56" s="196">
-        <v>0</v>
-      </c>
-      <c r="S56" s="202">
-        <v>11</v>
-      </c>
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A57" s="144"/>
+      <c r="A57" s="4"/>
       <c r="B57" s="4"/>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.3">
@@ -4357,14 +4241,6 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="4"/>
-      <c r="B66" s="4"/>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="4"/>
-      <c r="B67" s="4"/>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4375,7 +4251,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="H14 H51 H49 H46 H19 H28 H43" numberStoredAsText="1"/>
+    <ignoredError sqref="H14 H49 H47 H44 H19 H27 H41" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>